<commit_message>
feat: add fake header and error catch
</commit_message>
<xml_diff>
--- a/baike_spider/name.xlsx
+++ b/baike_spider/name.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,17 +464,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://cpc.people.com.cn/n1/2020/0729/c164113-31802331.html</t>
+          <t>https://www.baidu.com/</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>习近平倡导的“世界相处之道”</t>
+          <t>网页</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年07月29日10:14    来源：人民网-中国共产党新闻网	“中国始终支持多边主义、践行多边主义，以开放、合作、共赢精神同世界各国共谋发展。”国家主席习近平7月28日在亚洲基础设施投资银行第五届理事会年会视频会议开幕式上致辞。	习主席在致辞中多次强调“多边”，提出把亚投行打造成推动全球共同发展的新型多边开发银行、与时俱进的新型发展实践平台、高标准的新型国际合作机构、国际多边合作新典范等建议。	回头望，亚投行的筹建历程，体现了</t>
+          <t>设为首页关于百度About Baidu百度营销使用百度前必读意见反馈帮助中心有奖调研</t>
         </is>
       </c>
     </row>
@@ -486,17 +486,17 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtiNgIZG2NXzLV6aStUkQNc200728&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1&amp;allow_comment=1</t>
+          <t>http://tieba.baidu.com/</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>面对蛮横无理的美国，中国将作出坚定而理性的回应</t>
+          <t>贴吧</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+          <t>吧内搜索搜贴搜人进吧搜标签CJ即将开展，贴吧福利来啦点击抢签名照等大奖！带你玩转penbeat吧宅王之王争霸赛！北京电影节8月底举办茶杯头将登陆PS4吧友们的电竞梦想聚集地风靡全球的烧脑社交桌游！书吧读书使人进步2305351280195武汉吧武汉加油！中国加油！198611340593680钢铁是怎样炼成的吧3219小王子吧35764百年孤独吧27538史记吧28002汉书吧19401资治通鉴吧38145封神原著吧12275战国策吧5475论语吧61978三国演义吧267723水浒传吧190872西游记吧196865©2020 Baidu使用百度前必读贴吧协议隐私政策投诉反馈信息网络传播视听</t>
         </is>
       </c>
     </row>
@@ -508,17 +508,17 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtiD2VZIZfTk1LBKyC0vY1r200728&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1&amp;allow_comment=1</t>
+          <t>https://zhidao.baidu.com/</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>美媒：若美中关系恶化，美国多领域将受严重打击</t>
+          <t>知道</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+          <t xml:space="preserve">总有一个人知道你问题的答案解决个问题知道须知我的财富值0--我的现金0下载百度知道APP在APP端-任务中心提现我知道了--累计完成个任务10任务略略略略…50任务略略略略…100任务略略略略…200任务略略略略…您的帐号状态正常感谢您对我们的支持京ICP证030173号-1   京网文【2013】0934-983号            ©2020Baidu  使用百度前必读  |  知道协议  </t>
         </is>
       </c>
     </row>
@@ -530,17 +530,17 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtiMqJwgEujzLCkup3mY59a200728&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1&amp;allow_comment=1</t>
+          <t>http://music.baidu.com/</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>白宫抗疫表现到底怎样？</t>
+          <t>音乐</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+          <t>微信扫一扫随时关注音乐圈微信扫一扫随时关注音乐圈微信扫一扫随时关注音乐圈</t>
         </is>
       </c>
     </row>
@@ -552,17 +552,17 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://www.chinanews.com/gn/2020/07-29/9250801.shtml</t>
+          <t>http://image.baidu.com/</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t xml:space="preserve">在不确定性中创造确定性 </t>
+          <t>图片</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Ц──Ц──7Ф°┬28Ф≈╔О╪▄Д╦╜Е┘╠Д╦╜Е╓╝Ф■©Ф╡╩Е╠─Е╖■Е▒≤Ц─│Е⌡╫Е┼║И≥╒Е┴╞Ф─╩Г░├Е┬≤И╧╓Д╦▌Ф╛╖Г⌡÷Е╖■Е▒≤Д╪ Ф┴╖Х║▄Е┴╞Д╦╩Е╦╜Д╦°Е╦┐Г╫≈Е╓╚Ф√╞Е÷╨Ф√╞Д╩╔Х╖├И╒▒Д╪ Х╝╝Е╫╒Е╪▐Е┘╠Е░▄Д╦╩Ф▄│Г╛╛Е┘╚Ф╛║Д╦╜Ф╛╖Г╩▐Х╢╦И╚≤Е╠┌Е╞╧Х╞²Ц─┌Е▐▄Ф√╧Е⌡╢Г╩∙Б─°Е╪─Е░╞Е░▌Г√╚Ф┐┘Ф≈╤Д╩ёД╦╜Ф╛╖Е░┬Д╫°Ф√╟Е╠─И²╒О╪▄Е╪∙И╒├Е┘╗Г░┐Г╩▐Ф╣▌Г╗ЁЕ│╔Е╓█Х▀▐Е╒·И∙©Б─²Д╦╩И╒≤</t>
+          <t>抱歉，Safari不支持拖拽识图。 请保存图片到本地，通过本地上传或在搜索框粘贴图片url进行识图。IE9及以下版本浏览器不支持识图功能， 请升级浏览器或使用Chrome、QQ、搜狗浏览器进行识图</t>
         </is>
       </c>
     </row>
@@ -574,17 +574,17 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>http://m.top.cnr.cn/bdxw/20200729/t20200729_525185435.html</t>
+          <t>http://v.baidu.com/</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>考生因系统崩溃错过一本志愿填报？官方回应</t>
+          <t>视频</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t xml:space="preserve">女孩遭男子尾随 男子：我想睡你女子报复前男友 结果被炸飞忍者猫？胖猫空翻网友惊呆　　7月27日，一则“高考生因系统崩溃错过一本志愿填报”的消息引发关注。　　刚刚，回应来了。　　官方：填报期间系统一直正常　　今天上午，陕西省教育考试院网站发布“关于2020年陕西省高考志愿填报系统运行情况说明”，志愿填报期间系统一直工作正常。　　声明指出：　　2020年陕西省普通高校招生第一次志愿填报于7月24日12：00开始，7月27日12:00结束，共72小时，与往年时长相同。　　本次填报提前批次、单设本科批次、本科一批、普通高校职业教育单独招生志愿，共有122455人填报志愿（去年同期119557人）。　　</t>
+          <t>您预约的即将开始播放，去观看直播 &gt;&gt;伊拉克：新增病例维持高位国内再次全面宵禁美国多地抗议种族歧视暴力执法活动持续联邦人员对波特兰抗议者使用暴力逃离洪水后要警惕“失温”体温降至35℃以下会有生命危险跟踪50公里影帝式碰瓷网约车6人团伙碰瓷诈骗6000元内蒙古6名初中毕业生溺水出动80多人救援 2人获救4人溺亡欧洲多国采取措施限制民众前往西班牙五辆重型卡车进入美国驻成都领事馆大木箱被吊装在车上韩国大邱市长当众下跪磕头感谢医护人员深圳一女子寄件与快递员厮打快递公司回应绝了疾控提醒去草原不接近野生动物更不能食用！1重启之极海听雷992.1万2二十不惑975.1万3乘风破浪的姐姐952.3万4三十而已</t>
         </is>
       </c>
     </row>
@@ -596,17 +596,1531 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://www.baidu.com/duty/wise/wise_secretright.html</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>隐私策略</t>
-        </is>
-      </c>
+          <t>http://baijiahao.baidu.com/s?id=1673505882709386771</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr">
         <is>
-          <t xml:space="preserve">                百度公司非常重视用户信息的保护，在使用百度公司的所有产品和服务前，请您务必仔细阅读并透彻理解本声明。一旦您选择使用，即表示您认可并接受本条款现有内容及其可能随时更新的内容。            百度公司（本隐私保护声明中指北京百度网讯科技有限公司及其关联公司，以下亦称“我们”）非常重视用户个人信息及隐私权的保护， 因此我们制订了涵盖如何收集、存储、使用、共享和保护用户信息的隐私政策。我们希望通过本百度公司隐私权保护声明（以下亦称“本隐私政策”）向您清晰地介绍我们对您个人信息的处理方式，本隐私政策与您使用百度公司的产品和/或服务息息相关，请您在使用百度公司所有产</t>
+          <t>AI财经社文 | AI财经社 仉泽翔编辑 | 鹿鸣猝不及防，比特币突然迎来小阳春。据全球币价网站CoinMarketCap，7月26日，比特币短暂冲上10000美元高位后，7月27日，比特币再次冲高，最高点达到11386美元，截至发稿前，单价仍报10980美元。这是自6月以来，比特币首次突破10000美元。比特币的世界里，暴涨暴跌总是相伴，3月，比特币一度暴跌至4000美元以下，但也在2月、5月和6月三次叩击1万美元大关。行情的火热离不开资金的助攻。欧科云链OKLink数据显示，7月20日至 7 月 26 日，比特币链上活跃度持续上升，362.89万个比特币参与交易。其中链上活跃地址数总计 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtiV3hPGt5OdVURMaw5oCwF200727&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>微视频丨抗洪一线 党旗飞扬</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/n1/2020/0729/c40531-31802344.html</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>习近平对亚投行提出四点“新”期望</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年07月29日10:18    来源：人民网-理论频道	人民网北京7月29日电 (万鹏、任一林)“亚投行朋友圈越来越大、好伙伴越来越多、合作质量越来越高，在国际上展示了专业、高效、廉洁的新型多边开发银行的崭新形象。”国家主席习近平28日在亚洲基础设施投资银行第五届理事会年会视频会议开幕式上致辞，向会议表示祝贺，积极评价亚投行不断发展壮大，指出亚投行应该成为促进成员共同发展、推动构建人类命运共同体的新平台。	人民网・中国共产党新闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtiVJld4pdRgJiWbFQ8YYkN200728&amp;fromapp=cctvnews&amp;version=727</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>食为政首</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtiABGlcLL7Ii3vKOysRCIc200728&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1&amp;allow_comment=1</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>蓬佩奥称中国违反国际法 外交部回应</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtitYpIoRCVreJfcpmGyI74200728&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1&amp;allow_comment=1</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>《澳门日报》发表社评称美欲挑起新冷战难得逞</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>http://www.xinhuanet.com/world/2020-07/29/c_1210725542.htm</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>蓬佩奥这锅谎言“大杂烩”真馊</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　　近日，美国国务卿蓬佩奥发表涉华政策演讲，恶毒攻击中国共产党和中国社会制度，鼓噪世界联合起来“改变中国”。通篇演讲罔顾事实、颠倒黑白，充斥着意识形态偏见和冷战思维的霉馊味，是一锅政治谎言的“大杂烩”。　　这是一些美国政客针对中国，有计划进行的又一轮攻击和抹黑。谎言背后是疫情应对不力甩锅推责的政治算计，是对外示强扭转竞选颓势的党派私利，是打压孤立中国、维护美国绝对霸权的战略图谋。　　谎言翻炒千遍还是谎言，在真相面前不攻自破。中国共产党得到人民群众的衷心拥护和坚定支持，党民关系无惧挑拨。坚持走中国特色社会主义道路是历史和人民的选择，也是实践证明的正确选择。美方改变不了中国，中国也无意挑战或取代美</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>http://www.xinhuanet.com/politics/2020-07/29/c_1126299210.htm</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>传统产业上“云”记</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">　　新华社上海7月29日电　题：“疫情期间，我在线上卖出15万个垃圾桶”——传统产业上“云”记　　新华社记者周琳　　“海外订单还在的时候，我们的人没回来；等我们工人回来时，海外疫情起来了，外贸订单要么被取消、要么被搁置。”台州黄岩华萍生活用品有限公司总经理周挺，描述了今年遭遇的尴尬。　　时至今日，海外的很多订单依然没有恢复，但这家过去以外贸为主的“中国制造”企业，已经通过及时调整策略、加强“上云”售卖的方式，恢复了元气。今年上半年，公司各类产品在电商平台同比销量翻倍，带动营收同比增长30%，外贸类比重降到25%左右。　　华萍成立于1992年，早期生产日用塑料制品，如今产品已经覆盖厨房用品、垃圾</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/5e93e2/3zFdHQxFNYq?agt=8</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>澳美联合声明对中国进行无端指责和攻击 外交部回应</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t xml:space="preserve">【环球时报-环球网报道 记者 张卉】澳美日前双部长会期间发表联合声明，在涉及香港、新疆、南海等问题上对中国无端指责和攻击。对此，中国外交部发言人汪文斌在29日的例行记者会上表示，中方注意到美澳举行的外长和防长的”2+2”磋商。一段时期以来，美澳两国渲染炒作所谓的中国威胁，在一系列的问题上对中国进行污蔑抹黑，对此中方表示强烈不满，坚决反对，也分别向美澳提出了严正交涉。汪文斌称，我们敦促美澳正确的看待中国，停止采取干预中国内政，损害中方利益的言行，为中美中澳关系发展创造有利条件。同时我们也敦促美澳两国能够为地区的和平稳定发展发挥建设性作用，而不是相反。版权作品，未经环球网 huanqiu.com </t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>http://app.cctv.com/special/cportal/detail/arti/index.html?id=ArtimrIABCWBEGbXBtnDA36v200728&amp;fromapp=cctvnews&amp;version=807&amp;allow_comment=1&amp;allow_comment=1</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>我驻英使馆驳斥英媒刊登抹黑中国和平利用外空的文章</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>查看更多评论请先下载客户端了解最新资讯和新闻</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/67c0c8/3zFdZc2YNZt?agt=8</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>欧盟针对香港国安法出台限制措施 外交部：严正交涉</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>7月29日，外交部发言人汪文斌主持例行记者会。 有记者提问，28日欧盟针对香港维护国家安全立法出台一系列措施，包括限制向香港出口敏感技术设备。中方对此有何评论？ 汪文斌表示，香港是中国的特别行政区，香港事务纯属中国内政，任何外国或组织无权干涉。欧方通过的有关举措，违反了不干涉别国内政这一国际关系基本准则，中方坚决反对，已向欧方提出了严正交涉。 他指出，香港国安法的制定和实施是为了弥补香港长期以来在维护国家安全方面的法律漏洞，目的是为了健全香港法制，使“一国两制”在法治的轨道上行稳致远，完全符合宪法和基本法，不仅有利于香港的长治久安和长期繁荣稳定，也有利于维护所有在港外国企业和人员的正当合法权益</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/c36dc8/3zFbhO71xo4?agt=8</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>澳大利亚外长:并非所有观点都与美一致 澳无意伤害对华关系</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>【环球网报道 记者 崔天也】“我们和中国的关系很重要，我们无意伤害与中方的关系。”当地时间28日，澳大利亚外交部长佩恩在与美国国务卿蓬佩奥联合举行的记者会上称，尽管澳大利亚与美国在许多方面都将继续合作，但该国并非在所有问题上的观点都与美国完全一致。她表示澳大利亚“无意伤害与中方关系”，但也不会做出违背该国利益的事。据英国路透社29日报道，尽管目前新冠肺炎疫情严重，但澳大利亚外交部长佩恩和国防部长雷诺兹仍飞到华盛顿，与美国国务卿蓬佩奥和国防部长埃斯珀举行了两天的“2+2”会谈，应对中国问题据报是双方会谈的一大重点。在28日的联合记者会上，蓬佩奥对澳大利亚表示“赞赏”，并称华盛顿和堪培拉将继续合作</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/c36dc8/3zFfcgI8lru?agt=8</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>李登辉怎样了?蔡英文看后不语 其妻离开半小时折返(图)</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>【环球网报道 记者 张丽媛】李登辉昨晚被传出“死讯”，随后李登辉办公室主任王燕军否认他病亡。今天（29日）上午，蔡英文、赖清德、苏贞昌一同前往台北荣民总医院（荣总）探望李登辉。综合台媒报道，今天下午，蔡英文与苏贞昌均被问及李登辉病情，二人均未透露。 蔡英文（图源：台湾《联合报》） 台湾“三立新闻网”报道称，苏贞昌今天下午出席活动前接受采访，被问及上午去探视李登辉的情况。对于李登辉病情，他回应称，应该由医疗团队来说明比较清楚。 媒体追问有跟家属提到什么？他声称，有向家属表示关心，对李登辉表示祝福。 台湾《联合报》报道称，蔡英文今天下午出席民进党中常会，面对相关提问，她仅挥手致意，并没有针对李登辉</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/87f17a/3zFhdeASJA2?agt=8</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>乌鲁木齐：无症状感染者转为确诊病例的比例较大</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>7月28日，新疆新增本土确诊病例89例。7月29日，乌鲁木齐市政府副秘书长尚玉岚在发布会上介绍，随着病程推进，一些处于潜伏期的无症状感染者陆续出现临床症状，或CT检查出现新冠肺炎影像表现，成为确诊病例。所以今天新报告的确诊病例中，无症状感染者转为确诊病例的比例较大，达到了43例，现有无症状感染者数量有所下降。感谢您的反馈，我们将会减少此类文章的推荐</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/45075c/3zFgXFGDNIT?agt=8</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>吉林省委对贺电所作《平安经》有关问题进行调查</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>7月29日，吉林省委决定，成立由省委政法委牵头，省纪委监委、省委宣传部等部门组成的联合调查组，对吉林省公安厅党委副书记、常务副厅长贺电所作《平安经》有关问题进行调查核实。 感谢您的反馈，我们将会减少此类文章的推荐</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/b1c82f/3zFdFvNIQun?agt=8</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>7月"空台"已成定局!今年第3号台风"森拉克"又要"难产"?</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>中国天气网讯 今天，已经是7月29日了，离7月份正式画上句号还有不到三天，有一个不知道算好消息还是坏消息的“消息”要跟华南沿海小伙伴们宣布一下：今年7月份“空台”基本已成定局，是的，7月份不会有台风生成和影响我国了。不过，在即将到来的八月初，西北太平洋上已经有几个小“扰动”在蠢蠢欲动了，它们中或许有一个会在8月1日到8月2日前后影响我国华南沿海一带，然而……它是不是能成为今年第3号台风“森拉克”，目前还是个未知数，有可能只是一个热带低压。看了上面那一大段，小朋友们，你们是不是生出了很多问号？“森拉克”现在在哪？热带低压和台风有什么区别？热带低压会给华南沿海带来很强的风雨吗？不要着急，我们贴心的</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673509755490716337&amp;wfr=content</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>高福:我已接种实验型新冠病毒疫苗 作为科学家必须要勇敢</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>上传客户端关注动态原创 | 2.4万次播放· 发布时间：2020年7月29日 3858  1 504  1 564  2 3.9万  22 2493  18 32  0 73  0 34  0 2612  0 4.1万  28</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673527939989553091</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>落马副部被开除党籍后为何按四级调研员确定退休待遇？</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>新京报7月28日，河北省原省委常委、副省长张和因严重违纪违法受到开除党籍处分，按四级调研员确定其退休待遇；收缴其违纪违法所得。张和被开除党籍后为何按四级调研员确定其退休待遇？7月29日，中央纪委国家监委网站刊发《首个公开通报适用政务处分法给予处分的中管干部案例解析》。文章称，张和是政务处分法自今年7月1日施行后，首个公开通报适用政务处分法有关规定给予处分的中管干部案例。今年4月29日，中央纪委国家监委网站通报，张和接受中央纪委国家监委纪律审查和监察调查。3个月之后，审查调查认定，张和严重违反党的组织纪律、廉洁纪律并构成职务违法，性质严重，影响恶劣，应予严肃处理。张和在其退休已近10年时被查处，</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/24d596/3zFg91eUAoD?agt=8</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>香港修例风波共9216人被捕 青年学生占四成</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>香港警方今日（29日）公布，截至6月30日，共9216人在修例风波中被捕。当中有3725名学生，占全部被捕人40.4%，而大专学生和中学生分别占5成半和4成半。警方已检控1972人，当中被控暴动罪的有653人。须承担法律后果的有252人，包括被判签保守行为的有108人、被定罪的有141人，涉及罪行包括暴动、非法集结、刑事毁坏、侮辱国旗、伤人、袭警及藏有攻击性武器等，有57人已被判监禁，刑期由2星期至4年不等。大部份案件的司法程序正在进行中。另外，有16人经警司警诫处理。 香港警方表示，回顾修例风波已发生超过一年，去年6月起，暴力情况不断升级，去年11月发生“1111”马鞍山暴徒火烧人及“111</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/0c789f/3zFdg9GmhEC?agt=8</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>美政客炮制“中美接触失败论” 外交部:这是不尊重历史</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>7月29日，外交部发言人汪文斌主持例行记者会。澎湃新闻记者提问，还是关注到中美关系，美国国务卿蓬佩奥近日在尼克松总统图书馆发表讲话称，美与中国盲目接触的旧政策已经失败，中方没有像美方预期那样发生改变。你对此有何评论？ 汪文斌表示，近期，蓬佩奥等一些美国政客四处炮制所谓的“中美接触失败论”和“美国改造中国失败论”，针对这些论调，中方已经阐明了有关立场。这里，我再强调几点。 第一，所谓“中美接触失败论”不尊重历史、不符合事实。中美恢复交往和建交近50年来，中美双边各领域交流和合作不断拓展和深化，两国人民从中受益良多。据统计，中美经贸关系支撑美国国内260万个就业岗位，超过了7.25万家美国企业在华</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/536b97/3zFi1EYZ1Nt?agt=8</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>特朗普抱屈:都在抗疫,为什么认可福奇却不喜欢我?</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>约翰斯·霍普金斯大学当地时间7月28日公布的数据显示，美国新冠确诊病例已超过435万例，更惊人的是，单日新增死亡病例近1600人，为两个多月以来最高纪录。 当天，美国总统特朗普在白宫召开记者发布会，在回答提问时“坦诚”地反问，安东尼·福奇等专家和自己一样在做抗疫工作，为什么他们就那么受人推崇，却没人喜欢自己？ 他自己得出的结论是，性格不讨喜。 3月29日，美国总统特朗普（右）和美国国家过敏症和传染病研究所所长安东尼·福奇出席记者会。新华社/路透 “喜欢他却不喜欢我 这事很奇怪啊” 在当天的白宫记者会上，有记者问特朗普，对那条他说福奇误导了美国的推文被推特删掉这事，怎么看？ 特朗普一如既往长篇大</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/0c789f/3zFhvJblA7y?agt=8</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>拜登的副手候选人有哪些？美媒：少数族裔女性是热门</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>当地时间7月28日，美国前副总统、推定的民主党总统候选人拜登宣布，他将在8月的头一周里宣布自己在2020年大选中的竞选搭档，即副总统人选。 早在今年3月，拜登就承诺将拣选一位女性作为自己的搭档，并强调“有很多女性有资格在未来当选总统”。眼下离拜登首次作出表态已经过去了整整五个月，他现在觅得了哪些中意人选呢？ 职业检察官成头号热门 卡马拉·哈里斯 美国有线电视新闻网（CNN）7月23日发布了最新一版的每周拜登搭档排名表，其中最有希望成为拜登副手的是加利福尼亚州参议员卡马拉·哈里斯（Kamala Harris）。 哈里斯现年55岁，有一半非裔血统，她的父亲是牙买加人，母亲则来自印度。自上世纪90年</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673539156865638638&amp;wfr=content</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>现场直击！伊朗革命卫队围攻夺取“美航母”</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>上传客户端关注动态原创 | 46次播放· 发布时间：2020年7月29日 224万  1382 2.1万  5 171  0 9.9万  14 5.4万  14 29  0 8133  1 1065  0 2886  0 1423  1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/9f1f03/3zFh3SBHVkN?agt=8</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>纽约警察逮捕时将一女示威者强行塞入车中 美媒:真像绑架</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>【纽约警察逮捕时将一女示威者强行塞入车中，美媒：“手段真像绑架”】据《华盛顿邮报》7月29日报道，美国纽约一女子被警察“绑架”强行塞进车中，引发现场民众大声抗议。一段视频显示，几名便衣警察将一名女子强行塞进一辆没有警方标识的面包车后座，现场有不少围观者大声抗议，并试图帮助被逮捕的女子，但都被警察阻拦喝退，无法上前。这段视频在社交网络上传播后，遭到众多网友质疑，有网友怒斥“这样的逮捕，简直是光天化日之下的绑架”。《华盛顿邮报》也刊文称，“纽约警察抓示威者的手段真像绑架”。但也有网友表示，这并不是绑架，而是对那些有逮捕令或犯了重罪的人使用的方法。纽约警察局也在推特发布声明称，该女子曾在5起事件中破</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673517068719965167&amp;wfr=content</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>韩国植物园立安倍下跪谢罪雕像 日方表示强烈不满</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>上传客户端关注动态616次播放· 发布时间：2020年7月29日 420  0 69  0 536  8 0次播放  0 8097  0 962  0 2331  0 136  0 4.3万  6 24  0</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/24d596/3zFeOsSVNWg?agt=8</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>俄罗斯新增5475例新冠肺炎确诊病例 累计超82万例</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>据俄罗斯新冠病毒防疫官网发布的信息，截至莫斯科时间7月29日10时45分，过去24小时俄罗斯新增5475例新冠肺炎确诊病例，累计确诊828990例。新增治愈病例8116例，累计治愈620333例。新增死亡病例169例，累计死亡13673例。 首都莫斯科市新增确诊病例671例，累计确诊病例239986例。 目前全俄已累计进行了约2750万次新冠病毒检测，过去24小时共完成检测24.2万次，医学隔离观察的病例增加至26万人。（总台记者 顾鑫） 感谢您的反馈，我们将会减少此类文章的推荐</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/67c0c8/3zFeiCLAHG6?agt=8</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>北京：28日新增1病例 系27日确诊病例女婿</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>7月29日，北京市第162场新冠肺炎疫情防控工作新闻发布会召开。北青-北京头条记者从发布会现场了解到，北京市疾控中心副主任庞星火通报新增确诊病例和流行病学调查情况。7月28日0时至24时，北京新增大连市疫情关联病例1例，为7月27日确诊的大连市疫情关联病例的家庭成员。 某男，34岁，现住昌平区天通苑北街道西三区。7月23日下午，被告知其岳母为大连市无症状感染者的密切接触者后，一家人开始居家隔离，其岳母被转送到集中隔离点进行观察；7月27日，其岳母确诊后，该病例作为密切接触者由120救护车转送至集中隔离点进行医学观察，经核酸检测结果为阳性，随后由120救护车转运至昌平区医院就诊，体温38.1℃，</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673516604010791574&amp;wfr=content</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>林郑月娥亮相防疫短片 向全香港发出坚定呼吁</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>上传客户端关注动态原创 | 1.7万次播放· 发布时间：2020年7月29日 5126  5 3121  0 5719  3 23万  22 10万  157 2483  0 115  0 531  0 3.8万  28 3084  2</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/f60808/3zFT8LkXHTJ?agt=8</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>大连新增确诊8人</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>7月29日上午10时，大连市人民政府新闻办公室举行大连市新冠肺炎疫情防控工作第二十四次集中发布。 会上通报：截至7月28日24时，大连新增新冠肺炎确诊病例8人，均由无症状感染者转为确诊病例，3人为凯洋海鲜公司员工，一人为凯洋海鲜公司员工接触者，2人为大连湾街道居民，2人为确诊病例密切接触者。新增无症状感染者4人：其中，1人为凯洋海鲜公司员工，3人为确诊病例或无症状感染者的密切接触者。 累计确诊病例52例，其中46人普通型病例，3人轻型病例，3人为重型病例，30人为凯洋海鲜公司员工，9人为凯洋海鲜公司员工的接触者，9人为大连湾街道居民，4人为确诊病例或无症状感染者的密切接触者。 7月29日上午，</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/9bd673/3zFS9OAivBr?agt=8</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>大连30例确诊为大连凯洋海鲜公司员工</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>7月29日消息，大连疫情防控新闻发布会通报：自7月22日以来，大连累计确诊新冠肺炎病例52例，其中30人为大连凯洋海鲜公司员工，9人为大连凯洋海鲜公司员工接触者，9人为大连湾街道的居民，4人为确诊病例或无症状感染者密接。所有确诊病例均在医院集中隔离治疗，目前病情稳定。 感谢您的反馈，我们将会减少此类文章的推荐</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/a4d1ef/3zFRoQje64w?agt=8</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>三部门：因疫情造成游客滞留 新增食宿费用游客承担</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>近日，最高法、司法部和文旅部发布《关于依法妥善处理涉疫情旅游合同纠纷有关问题的通知》，通知提到，因疫情影响旅游者人身安全，旅游经营者应当采取相应的安全措施，因此支出的费用，由旅游经营者与旅游者分担。因疫情或者疫情防控措施造成旅游者滞留的，旅游经营者应当采取相应的合理安置措施，因此增加的食宿费用由旅游者承担，增加的返程费用由旅游经营者与旅游者分担。感谢您的反馈，我们将会减少此类文章的推荐</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/0c789f/3zFdmB5Mrf2?agt=8</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>山西洪洞一女生遭人围堵被扇耳光18次 县教育局:正在处理</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>白衣女生被三人扇耳光，踢踹。爆料者提供 针对山西省临汾市洪洞县一位女生遭人围堵扇耳光事件，7月29日，洪洞县教育局办公室一名工作人员告诉澎湃新闻，目前涉事学校和洪洞县教育局安全股的工作人员正在负责处理。“学生家长已经来了”。 29日，洪洞县的李由（化名）向澎湃新闻反映，7月15日，他从洪洞县家乡群里看到有人在传播一段女生遭人围堵扇耳光的视频。根据视频中的口音，他判断事发地点应该在洪洞县。 白衣女生被三人扇耳光，踢踹。爆料者提供 李由向澎湃新闻提供的视频画面显示，一名身穿白色上衣的女生被一名身穿黑色上衣的男生和两名身穿黑色上衣的女生围堵在墙边。其中一名身穿黑色上衣的女生上前连续打了白衣女生多个耳</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/569e98/3zFdibyqM9a?agt=8</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>“苦等十年的回迁房要穿6道门且第29层没电梯”续:可换房</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>云南昆明市西山区马街摩尔城 小区业主邓女士表示 这个楼盘烂尾了十年 最近终于可以收房 没想到却抽到29楼的奇怪户型 要想进家门 得穿过6道防火门 电梯不能直达 甚至都没有29层的按键 类似邓女士的情况 在这个回迁房小区里 至少有六户 收房难，进家门更难 不仅回家要过六道门 层高最低处也只有2米无法住人 邓女士说，经过了十年的等待，7月初，马街摩尔城的回迁户开始摇号抽签，她家抽到了11栋29楼的一套房子。但看房时，他们才发现：29楼居然没有直达的电梯。邓女士：“我们要下半层楼或者到28层的话上半层楼。出了电梯后到安全出口，我们打开门，这是第一道，来第二道，我们要下去又得打开（防火门），是不是很奇</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>http://m.top.cnr.cn/bdxw/20200729/t20200729_525185435.html</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>考生因系统崩溃错过一本志愿填报？官方回应</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">女孩遭男子尾随 男子：我想睡你女子报复前男友 结果被炸飞忍者猫？胖猫空翻网友惊呆　　7月27日，一则“高考生因系统崩溃错过一本志愿填报”的消息引发关注。　　刚刚，回应来了。　　官方：填报期间系统一直正常　　今天上午，陕西省教育考试院网站发布“关于2020年陕西省高考志愿填报系统运行情况说明”，志愿填报期间系统一直工作正常。　　声明指出：　　2020年陕西省普通高校招生第一次志愿填报于7月24日12：00开始，7月27日12:00结束，共72小时，与往年时长相同。　　本次填报提前批次、单设本科批次、本科一批、普通高校职业教育单独招生志愿，共有122455人填报志愿（去年同期119557人）。　　</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>http://m.top.cnr.cn/bdxw/20200729/t20200729_525185434.html</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>秦淮河大坝"肚子"建餐厅,9人被处理!这些问题仍需关注</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>女孩遭男子尾随 男子：我想睡你女子报复前男友 结果被炸飞忍者猫？胖猫空翻网友惊呆　　今年入汛以来，受长江大流量来水和强降雨影响，长江下游南京段持续超出警戒水位，秦淮河水位超高，当地一度启动防汛一级应急响应。有群众向中国之声反映秦淮河杨家圩大堤被向内挖空十几米，如此严峻的防汛形势之下，多家餐厅、酒吧在大坝“肚子里”营业，可能对堤防造成安全隐患。　　图为大坝顶部，右侧红圈内为餐厅　　总台央广记者独家调查报道后，秦淮河杨家圩大堤内部违规建设、经营的酒吧、餐厅等已经停业，有施工人员拆除门脸。　　图为工作人员正在拆除</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>https://3w.huanqiu.com/a/14a2fb/3zFdmQl8p6J?agt=8</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>接受管理服务对象"感情投资"241万余元,为何被认定受贿罪?</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>图为六盘水市纪委监委审查调查人员研判李晓忠案案情。 特邀嘉宾 周 谊 六盘水市纪委监委第八审查调查室主任 高永松 六盘水市纪委监委案件审理室三级主任科员 姜 黎 钟山区人民检察院检委会专职委员 谢 鸿 钟山区人民法院刑庭负责人 编者按 与典型的受贿形式“一事一贿”不同，本案中李晓忠受贿总额近一半没有对应的具体谋利事项，为何也认定其构成受贿罪？判决书中多次出现“感情投资”一词，何为“感情投资”？接受“感情投资”在什么情况下构成受贿罪，又在什么情况下构成违纪，实践中怎么区分把握二者？李晓忠受贿241万余元获刑7年，法院在量刑时考虑了哪些因素？我们邀请相关单位工作人员对这些问题进行分析。 基本案情：</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673521267977026089</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>疯狂"长寿药"调查:国外"镀金"卖天价 有消费者直接买原料吃</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>新京报60粒，9.6克，售价却从2000元直至过万不等。似乎一夜之间，在小圈层蹿红已久的“长寿药”，以一种轰动的方式进入大众视野。“长寿药”吸引的不只是想要长寿的人：该领域代表上市公司金达威11天创下8个涨停，正在印证着资本的癫狂。    嗅觉敏锐的投资人姚远（化名）注意到了“长寿药”NMN领域近期的爆火趋势，一份在业内流传、看好该领域的研报更令他跃跃欲试。经过选择，过去从来不买保健品的姚远决定亲身试药，并网购了一款美国品牌的NMN产品。   “吃到第四天了，暂时没什么感觉。”姚远说。   尽管如此，“长寿药”的“潘多拉魔盒”已经开启。“李嘉诚这些名人都在吃，还投资”“我们是明星代言，老客户都</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673539295675471050&amp;wfr=content</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>武汉协和医院一护士坠楼 疑曾与主任起冲突</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>上传客户端关注动态原创 | 1.6万次播放· 发布时间：2020年7月29日 334  0 3.4万  27 15  0 27  0 1  0 1654  22 3  0 4220  2 1474  0 5929  4</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673543480247192349&amp;wfr=content</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>实拍女德班雷人教学现场 官方：介入调查 责令停改！</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>上传客户端关注动态原创 | 244次播放· 发布时间：2020年7月29日 24  0 4.5万  114 27万  216 14万  34 332  0 7  0 2.1万  2 46  0 9477  35 15  0</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E4%B9%A0%E8%BF%91%E5%B9%B3%E5%9C%A8%E4%BA%9A%E6%B4%B2%E5%9F%BA%E7%A1%80%E8%AE%BE%E6%96%BD%E6%8A%95%E8%B5%84%E9%93%B6%E8%A1%8C%E7%AC%AC%E4%BA%94%E5%B1%8A%E7%90%86%E4%BA%8B%E4%BC%9A%E5%B9%B4%E4%BC%9A%E8%A7%86%E9%A2%91%E4%BC%9A%E8%AE%AE%E5%BC%80%E5%B9%95%E5%BC%8F%E4%B8%8A%E8%87%B4%E8%BE%9E</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>习近平在亚洲基础设施投资银行第五届理事会年会视频会议开幕式上致辞</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E4%B9%A0%E8%BF%91%E5%B9%B3%E6%80%BB%E4%B9%A6%E8%AE%B0%E5%85%B3%E5%88%87%E4%BA%8B%E4%B8%A8%E7%BB%BF%E6%B0%B4%E9%9D%92%E5%B1%B1%E2%80%98%E9%87%91%E9%A5%AD%E7%A2%97%E2%80%99</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>习近平总书记关切事丨绿水青山‘金饭碗’</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E5%9C%A8%E4%BA%AC%E9%AB%98%E6%A0%A1%E6%96%B0%E7%94%9F%E6%8A%A5%E5%88%B0%E5%88%86%E6%89%B9%E5%88%86%E6%9C%9F%E8%BF%9B%E8%A1%8C</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>在京高校新生报到分批分期进行</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E5%A4%A7%E8%BF%9E30%E4%BE%8B%E7%A1%AE%E8%AF%8A%E4%B8%BA%E6%B5%B7%E9%B2%9C%E5%85%AC%E5%8F%B8%E5%91%98%E5%B7%A5</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>大连30例确诊为海鲜公司员工</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E7%99%BE%E5%A7%93%E5%86%92%E9%9B%A8%E9%80%81%E6%8A%97%E6%B4%AA%E6%88%98%E5%A3%AB%E7%86%9F%E9%B8%A1%E8%9B%8B</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>百姓冒雨送抗洪战士熟鸡蛋</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E8%88%AA%E7%A9%BA%E6%97%85%E8%A1%8C2024%E5%B9%B4%E6%89%8D%E8%83%BD%E6%81%A2%E5%A4%8D%E6%AD%A3%E5%B8%B8</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>航空旅行2024年才能恢复正常</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E7%A8%8B%E5%BA%8F%E5%91%98%E7%94%A8CPU%E7%83%A4%E8%82%89</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>程序员用CPU烤肉</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E9%98%BF%E5%B0%94%E5%8D%91%E6%96%AF%E5%B1%B1%E7%8E%B0%E7%B2%89%E7%BA%A2%E8%89%B2%E5%86%B0%E5%B7%9D</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>阿尔卑斯山现粉红色冰川</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E8%8B%B1%E6%94%BF%E5%BA%9C%E6%96%A5%E8%B5%8420%E4%BA%BF%E9%BC%93%E5%8A%B1%E6%AD%A5%E8%A1%8C%E9%AA%91%E8%BD%A6</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>英政府斥资20亿鼓励步行骑车</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>https://www.baidu.com/s?wd=%E7%BE%8E%E5%9B%BD%E9%A6%96%E4%B8%AA%E6%96%B0%E5%86%A0%E7%96%AB%E8%8B%973%E6%9C%9F%E4%B8%B4%E5%BA%8A%E5%90%AF%E5%8A%A8</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>美国首个新冠疫苗3期临床启动</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>问题反馈</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673457963672419498</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>孟晚舟案追踪：汇丰的“局”，华为的“据”</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>出行一客孟晚舟律师团队将辩护重点放在了两个地方：一是美加行政当局提供证据的可采纳性，二是美加当局是否滥用司法程序文 | 《财经》记者 谢丽容 周源  特约作者 李隐枫   编辑 | 马克加拿大当地时间7月23日下午，负责审理孟晚舟引渡案的加拿大不列颠哥伦比亚省高等法院的一个法庭（下称“加拿大法庭”）公开了华为最新提交的部分证据。这些证据回应了美国司法部的一个重要指控：孟晚舟欺骗了包括汇丰银行在内的银行，误导了他们对华为与Skycom公司真实关系的判断，这导致汇丰银行违反了美国对伊朗的制裁法规。孟晚舟律师团队提交的抗辩申请认为，美国司法部歪曲了事实，“对孟女士的案件记录进行了不适当的剪裁”，以“</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673509952626721031</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>贝壳出海，壳够“硬”吗？</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>BT财经V北京时间7月24日，多次否认IPO消息的贝壳找房终于向SEC递交了IPO文件，承销商包括高盛、摩根士丹利、华兴资本、摩根大通等。据悉，贝壳此次IPO寻求不超过30亿美元的融资，希望市场估值达到200亿美元。如果顺利，贝壳将是今年中国企业在美股最大规模的IPO，也将成为继腾讯音乐娱乐集团（TME）后第二家在美IPO融资规模超10亿美元的中国企业。贝壳D+轮融资后的市场估值已高达140亿美元（约1000亿人民币）。一位投资人在接受媒体采访时表示，贝壳的估值已经很高，他身边多家 PE 机构均表示“不会碰这家公司”。左晖的“全部家当“在招股说明书开头的信中，左晖称贝壳未受疫情影响按期递交IP</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673512533327576789</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>搜狗可能算不上什么“好商品”</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>钛媒体APP图片来源@视觉中国文丨互联网指北，作者丨大浅，编辑丨蒲凡腾讯向搜狗发出初步非约束性收购邀约，腾讯有意以9美元/ADS的价格收购搜狗剩余股份。当日晚间，搜狗发布公告证实了这一消息。随后，搜狗CEO王小川也发布朋友圈表示：“感谢腾讯公司对搜狗公司价值以及技术能力、产品创新能力的认可。接下来会对相关事宜进行认真的讨论和衡量，让搜狗能够持续为用户创造更大的价值。”随着相关消息的发酵，搜狗盘前涨超40%，最终收盘上涨48%，市值一夜之间飙涨了10.8亿美元。而与之对应，持股搜狗33.8%的搜狐股价也随之增长了近40%。其实，腾讯与搜狗的渊源由来已久。早在2013年，腾讯就通过投资获得了搜狗3</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673516756424203807</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2020过半，科技并购真的来了</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>甲子光年有路才能到山前。作者 | 王学琛编辑 | 火柴Q“十亿市值靠业务，百亿市值靠并购，千亿市值靠核爆业务+并购。”曾任立思辰战略管理与投资并购部总经理的丁建英在《兵临城下：中国上市公司并购风云》一书中总结中国企业“并购成长”逻辑。书中总结了1993年~2018年间，中国上市企业的并购案例。其中，上一个让人血脉喷张的大并购时期是2013~2016年：以BAT三巨头为主的中国互联网曾掀起一波又一波投资并购浪潮，美团、大众点评合并，携程、去哪儿合并，滴滴、快的合并，58、赶集合并等大并购案例也令人目不暇接。虽然后来的故事证明，成为寡头也并不意味着可以就此高枕无忧。但这些因并购诞生的新巨头，在之后</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673515447423859778</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>王小川不惑：裂土为王or腾讯封臣</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>盒饭财经作者 / 苗正卿来源 / 盒饭财经（ID：daxiongfan）天才少年王小川，已消失不见。站在你面前的，是中年人王小川。虽然有一张娃娃脸，但细节依然出卖了他：喝的咖啡变少，橙汁和热水被列入日常饮品；开始控制酒量，对命运也有些新思考。“命运可能是注定的。”在2018年《十三邀》的录制现场，王小川在许知远的追问下，略做思考后轻声回答。从他办公室一角可见端倪，王小川养了一缸鱼，他称之为“风水鱼”。不同人经过鱼缸，鱼会给出不同反应。有的人会让鱼睹之变色，而另一些人则无法让鱼提起兴趣。王小川审慎地说，“这鱼能看到外面”。看到有人经过，鱼在水中乱窜，这位年过40、身价近20亿元的搜狗CEO会露出</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673513371445849172</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>“鹅吞狗”的想象力：始于搜索框，终于生态圈</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>新浪科技来源：创事记欢迎关注“创事记”的微信订阅号：sinachuangshiji　文/杨泥娃来源： 电商在线（ID：dianshangmj）不确定“鹅吞狗”在生物界算什么地位，但在互联网圈是门划算的生意。7月27日晚，腾讯向搜狗发出初步非约束性收购要约，收购价在每股9美元左右，按照搜狗目前的流通股以及腾讯的持股情况来计算，腾讯收购搜狗的花费大概在147亿元左右。（消息一出，搜狗股价涨幅48%）搜狗CEO王小川随即在朋友圈对腾讯表达了感谢，搜狐董事局主席兼CEO张朝阳也表达了支持的态度。不仅全部售出了自己持有的6.5%股份，还将投票权也用来支持本次交易。基本可以确定，长达7年的“鹅狗狐”三角关</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673512643775060264</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>腾讯欲买走搜狗，背后的真实原因并非因为百度</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>新浪财经来源：星空财富今天腾讯和搜狗的联姻再度走上舆论风口。其实早在2013年，企鹅试图抢占搜索的市场份额，于是开始了寻找一只狗。于是企鹅找到了狗妈——搜狐。搜狗是搜狐公司的一款搜索引擎，更确切的说是一个产品。这些年大风大浪过后，搜狗还干的不错。企鹅也曾自己试图组建团队开发一个搜索引擎，事实证明没有这个基因，做不出像微信一样优秀的产品。企鹅也很少在江湖上再提起搜搜，搜搜去哪了呢？企鹅和狐狸一拍即合，注资4.48亿美元把搜搜装进了搜狗。作为一枚普通用户，我们平时在PC端找东西一般都用度娘；而找新媒体文章，我一般都会用搜狗。也就是说搜狗提供的是微信公众号内容全网搜索。而度娘不是没有技术，而是没办法</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673512251896340248</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>“迟钝”的王小川为何一直受到马化腾青睐</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>新浪科技来源：创事记欢迎关注“创事记”的微信订阅号：sinachuangshiji　文/马畅来源：笔记侠（ID：Notesman）原标题：搜狗王小川：不断对自己思考和定位　　在王小川眼里，做公司更像是在“做一个生命”，都要做两件事：第一，性状相对稳定；第二，可以自我复制。7月27日晚，腾讯公司发出初步非约束性收购要约，有意全资收购中国第二大搜索引擎公司搜狗，交易价格为每股9美元。随后，王小川在朋友圈回应：“感谢腾讯公司对搜狗公司价值以及技术能力、产品创新能力的认可。接下来会对相关事宜进行认真的讨论和衡量，让搜狗能够持续为用户创造更大的价值。”王小川曾说，他的性格中有一面是“面对世事变化懒得应对</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673469743777145530</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>携程退市求稳？</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>虎嗅APP出品 | 虎嗅大商业组作者 | 刘然题图 | 视觉中国正在自救的携程可能还是要考虑迈出“退市”这一步了。根据路透社的报道，携程正与潜在投资者就其从纳斯达克退市进行谈判，并且携程管理层已就私有化交易与多位金融和战略投资者进行了接触，其中包括私募股权公司和国内科技公司。不过消息人士也表示，有关携程退市的讨论尚处于早期阶段，可能会发生变化。对于此次传闻，携程回应虎嗅称不予置评。但从今年年初开始，已经不断有消息称包括百度、携程等在内的中概股巨头正在推进香港二次上市的进程，再看此次的传闻，听起来已经有几分为真。此时的携程，在与黑天鹅的抗争中还未赢得胜利，还要面临国际化的推进，即使退市回港，它所</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673439604364588635</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>马化腾二度搜索王小川</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>虎嗅APP虎嗅机动资讯组作品作者 | 胡展嘉题图 | 视觉中国搜狗要易主了。7月27日晚间，搜狗（NYSE：SOGO）表示收到来自腾讯的有意收购公司的初步非约束性要约。根据公告，腾讯拟收购搜狗全部已发行普通股，其中包括腾讯或其关联公司目前尚未持有的搜狗美国存托股票（ADS）所代表的普通股，收购价为每股普通股或美国存托股票9.00美元，支付方式为现金。也就是说，在这次收购完成后，搜狗将彻底姓“马”。受此影响，搜狗周一收盘价暴涨48%，报8.51美元。至此，马化腾离他的搜索小目标又近了一步。搜索这事儿，让腾讯又爱又恨对于搜索这件事儿，腾讯可谓执念颇深，甚至可以追溯到“远古”的PC时代。时间拉回20</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673513478310262336</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>比特币为何重回1万美元高点？</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>钛媒体APP图片来源@视觉中国文丨一本财经，作者丨棘轮 林格股票、黄金、比特币……7月以来，多种资产轮番上涨，吸引了投资者的眼球。7月26日晚间，比特币经历多日上涨后，冲上1万美元关口。“5位数的比特币回来了。”有玩家感慨。甚至有国外玩家开始“感谢上帝”，或者戏称“比特币治好了我的抑郁症”。一度暂停购入比特币的大户灰度投资，也恢复了对比特币的投资。但对于这次比特币上涨的原因，外界仍旧众说纷纭。尽管比特币本次上涨表现稳健，但仍有业内人士指出，比特币未来的走势并不明朗。在这个动荡不安的时代，比特币还会出现怎样的动荡？01、重回一万美元1万美元，是许多币圈玩家的心理门槛。而今，比特币正在站上这一门槛</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673510393585668326</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>腾讯收购搜狗：PC互联网江湖正落幕</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>钛媒体APP图片来源@视觉中国文丨itlaoyou-com，作者丨韩志鹏靴子即将落地。7月27日晚，搜狗公告称，已收到腾讯的初步非约束性要约，拟以每普通股或每美国存托股份9美元的价格收购搜狗；若完成交易，搜狗将成为腾讯的间接全资子公司，并从纽交所退市。消息放出，搜狗股价一路飙升。截止27日收盘，搜狗股价大涨48%，市值超过32亿美元，搜狐股价同样收涨近40%，二者股价均攀升至一年中最高点。对于收购，搜狗CEO王小川也回应称：会对相关事宜进行认真的讨论和衡量。生于PC时代，搜狗已经成立超过15年，其与腾讯、搜狐都称得上中国“老一辈”的互联网公司。而自腾讯入股搜狗以来，双方合作也已持续7年之久。七</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673500019768138286</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>影院开放首周：复工率接近50%</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>三言财经自7月20日至今，电影院恢复开放营业已经过去一周了。时隔半年，观众再次走进影院，“零点场”回归、电影节票一抢而光、多部国内外电影相继定档，电影市场逐渐热闹了起来，但也有一些影院，刚刚开放又面临暂停……一周时间里，全国影院复工进程如何？还能回到往日的火爆吗？资料图：7月24日，位于北京市朝阳区的一家电影院开始放映影片。 中新社记者 侯宇 摄超5000家影院复工，大连影院开了又关7月16日，国家电影局发布通知称，低风险地区在电影院各项防控措施有效落实到位的前提下，可于7月20日有序恢复开放营业。告别半年的“冰封”状态，电影院终于等到观众的到来。7月20日，第一批符合复工条件的电影院率先开门</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673486408367722301</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>滴滴的估值游戏</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>三言财经文/左岸来源：懂懂笔记（ID：dongdong_note）“一周之内，滴滴的两个独立品牌青菜拼车和花小猪面世，加上此前6月份内部出租车事业部、顺风车和同城货运的一系列动作，你能说和资本层面没有任何关系吗？”“8年拿了19轮融资，这200亿美元融资额里可是有阿里、腾讯、软银、高瓴和丰田等那么多互联网、VC以及车企巨头的身影，滴滴可以不着急，但这些股东呢？”谈及滴滴近日再次被传出IPO相关话题，几位业内分析人士如是说。近日包括《财新》等多家媒体报道称：滴滴已经开始与投行进行接触，IPO最快将在年内完成，上市地点为香港，目标估值超过 6000 亿港币（约合800亿美元）。对此，滴滴副总裁李敏</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673465675586572096</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>富士康“学徒”立讯精密准备切苹果代工蛋糕</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>新京报贝壳财经库克参观立讯精密。图片来源：立讯精密官网。 身着蓝色工装服的苹果CEO蒂姆·库克双眼凝视着生产线工人完成组装。由于部件过于精密，这名工人不得不侧脸看放大的屏幕，然后双手完成装配。工人手中的小玩意儿AirPods帮助苹果公司再度引爆全球购买狂潮，人们迫切地购买这款创新的入耳式无线耳机，甚至愿意等待数周。这是2017年12月的一天。这一年苹果已为耳机产品申请过了多个专利，并将生产交给了一家名为“立讯精密”的中国大陆工厂。蒂姆·库克到访的就是这家工厂位于昆山的生产基地。一张照片记录了当时的情景，而在他身旁的一位中年女子就是这家公司的老板王来春。这也是库克此次到访中国一系列行程中重要环节</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673465674428420320</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>滴滴恢复北京网约车跨城订单服务</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>新京报贝壳财经新京报贝壳财经讯（记者 陈维城）7月28日，滴滴方面介绍，滴滴在北京已恢复目的地为低风险地区的出京运营业务。同时，因疫情防控降级，防护膜安装站点及线下防疫消毒点将于7月31日全部下线。7月24日，北京市交通委员会发布相关通知称，按照市新冠肺炎疫情防控工作领导小组关于常态化疫情防控的有关要求，从发文之日起恢复本市出租车(含巡游车、网约车)、顺风车目的地为低风险地区的出京运营业务。据悉，北京疫情反弹后的6月16日，北京应急响应级别由三级提升到二级。6月20日，滴滴重新开放了防护膜安装点和线下防疫站点。滴滴方面介绍，恢复免费安装防护膜以来，滴滴在北京已为3024辆网约车免费安装了防护膜</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673509401331404181</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>黄金涨价背后</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>AI财经社文 | AI财经社 周享玥编 |鹿鸣（图源：视觉中国）“前浪”赚了多少钱？“是金子总会发光”，这是阿霁在面对不断上涨的金价时脑子里涌现出的第一想法。作为被此次金价暴涨眷顾的幸运儿之一，阿霁家的黄金存货不仅成功得以解套，还小赚了一笔，“目前大概还有2000克左右的金条吧，前几天看到价格涨到合适的心理价位了，就先以410元/克的价格出掉了一些，免得之后再跌”。阿霁口中“发光的黄金”还在持续疯涨中。7月24日，伦敦现货黄金一举突破1900美元关口；仅3天后，就成功越过2011年以来保持了9年的历史最高纪录1921.15美元/盎司，再创新高，当天收1942.64美元/盎司；7月28日早间，现</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673461020098084236</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>携程有必要退市吗？</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>AI财经社文 | AI财经社 刘雪儿编辑 | 孙静本文由《财经天下》周刊旗下账号AI财经社原创出品，未经许可，任何渠道、平台请勿转载。违者必究。老板梁建章的直播还没完事，携程便传出退市消息。7月28日，据路透社报道，携程正与私募投资公司、国内科技公司在内的财务投资者、战略投资者接触，计划筹集资金从纳斯达克退市。同时也不忘强调：携程退市讨论还处于早期阶段，可能会有变化。携程对此不予置评。路透社把原因归结为中美紧张局势加剧，以及新冠病毒对旅游业务的影响。在国内投资人李明奇看来，携程私有化的动机主要是未来在国内上市，“因为现在两地上市主要是H股+A股，或美股+H股，还没有美股+A股的先例。”不过李明</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>https://baijiahao.baidu.com/s?id=1673476618665539543</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>腾讯“利用”了递投名状的人</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>全天候科技收购搜狗，接管阅文，腾讯似乎越来越像阿里。它在下一盘怎样的棋？作者|吴健伟 编辑|罗丽娟马化腾又出手了，这一次是准备大手笔拿下搜狗。7月27日晚，搜狗发布公告称，收到来自腾讯的有意收购公司的初步非约束性要约，给出的收购价格是每股普通股9美元。交易一旦完成，搜狗将成为腾讯的间接全资子公司，同时从纽约证券交易所退市，成为一家私人控股公司。搜狗CEO王小川顺手推舟，随后在朋友圈感谢了腾讯对搜狗的认可，并表示会认真讨论和衡量。BT财经报道称，此次交易也已经获得了搜狐CEO张朝阳的支持。实际上，在此之前，腾讯已为搜狗第一大股东，持有搜狗39.2%的股份，为第一大股东；第二大股东搜狐持有搜狗33</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>http://baijiahao.baidu.com/s?id=1673505882709386771</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>比特币被判为“货币”，美国会割全球韭菜吗</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>AI财经社文 | AI财经社 仉泽翔编辑 | 鹿鸣猝不及防，比特币突然迎来小阳春。据全球币价网站CoinMarketCap，7月26日，比特币短暂冲上10000美元高位后，7月27日，比特币再次冲高，最高点达到11386美元，截至发稿前，单价仍报10980美元。这是自6月以来，比特币首次突破10000美元。比特币的世界里，暴涨暴跌总是相伴，3月，比特币一度暴跌至4000美元以下，但也在2月、5月和6月三次叩击1万美元大关。行情的火热离不开资金的助攻。欧科云链OKLink数据显示，7月20日至 7 月 26 日，比特币链上活跃度持续上升，362.89万个比特币参与交易。其中链上活跃地址数总计 5</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>http://news.baidu.com/</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>http://report.12377.cn:13225/toreportinputNormal_anis.do</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>http://report.12377.cn:13225/toreportinputNormal_anis.do</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>HTTP ERROR</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: fixed invalid url detection problem
</commit_message>
<xml_diff>
--- a/baike_spider/name.xlsx
+++ b/baike_spider/name.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,920 +459,3164 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>http://auto.sina.com.cn/newcar/index.d.html</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>新车</t>
-        </is>
-      </c>
+          <t>http://sports.people.com.cn/n1/2020/0810/c14820-31816333.html</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2020-08-07刚上市BEIJING-EU5车型频道2020-08-07刚上市几何C车型频道2020-08-08刚上市新宝骏RC-5车型频道2020-08-10刚上市哈弗H6车型频道2020-08-10上市领克02车型频道2020-08-10上市沃尔沃S90车型频道2020-08-13上市荣威ER6车型频道我们获得一组全新第三代奔腾B70尾部官图，新车采用了全新设计语言，溜背式的车尾十分运动。除此之外，该车掀背尾门、小鸭尾造型和贯穿...查看全文&gt;&gt;新车计划国产新车奔腾2020-08-10 14:44:19分享评论0我们从外媒获悉，日产全新一代GT-R将于2023年亮相，新车预计采用油电混</t>
+          <t>登录人民网通行证    立即注册忘记密码？本报记者  范佳元					　　8月8日，球员在篮下拼抢。当日，广东队以88∶85战胜北京队，从而以2∶1的总比分淘汰对手，晋级本赛季中职篮总决赛。					　　新华社记者 李紫恒摄	　　核心阅读	　　2019―2020赛季中职篮总决赛将于8月11日晚开赛，比赛采取三战两胜制。一边是第十五次晋级总决赛的上赛季冠军广东队，一边是第八次闯入总决赛的辽宁队，期待两队为球迷奉献更加精彩的比赛。	　　	　　8月8日，2019―2020赛季CBA（中国男篮职业联赛）季后赛半决赛全部结束，晋级总决赛的是同样有着丰富经验和强大阵容的辽宁队和广东队。	　　总决赛将于8月</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>http://m.sina.com.cn/m/sinaopencourse.shtml</t>
+          <t>http://history.people.com.cn/GB/198819/index.html</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>新浪公开课</t>
+          <t>国家人文历史</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>新浪公开课iPad、iPhone、Android新版客户端上线，界面设计更美观，内容分类更清晰，视频播放更流畅，还新增一键分享和离线观看功能。新特性：①全新界面，结构更清晰；②增加一键分享到新浪微博，微信及微信朋友圈 ；③增加离线观看功能，随时随地观看课程视频。一起体验掌上学习风暴。最新版本：2.0.2版 [2015-02-02更新]数千节不断更新的国内外一流大学讲座及名人演讲视频，涵盖九大学科，配有中英文双语字幕集结全球各界精英，用短小精干的18分钟演讲改变世界，500多场讲座你绝对一个都不想错过与七十五万活跃新浪微博粉丝共同关注公开课，互通有无，寻找志同道合的学习同路人iphone、ipa</t>
+          <t>人民网首页|文史频道|网站地图    1978年12月，党的十一届三中全会开启了改革开放的新时期,至今已经走过了40年的风雨岁月。在这40年中，我国发生了翻天覆地的变化，GDP总量从1978年的3650亿元跃升到2017年的82万亿元，稳居世界第二，经济实力、科技实力、国防实力、国际影响力不断提升。从改革开放40年来的各项数据看，无论是经济增长还是国民生活，中国都取得了令世界惊叹的成就，正在以不可阻挡之势，迈向发达国家行列。不同于小国，在中国这样一个十多亿人口的大国，面临的问题非常复杂，要实现党的十八大报告提出的全面建成小康社会的目标绝非易事。40年的强国之路有着太多重要节点，我们有选择地讲述</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/gov/2020-08-10/doc-iivhvpwy0171573.shtml</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr"/>
+          <t>http://bbs1.people.com.cn/board/2.html</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>深入讨论</t>
+        </is>
+      </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：31省份最低工资：桂闽青已上调 京津沪暂缓调整　　中国网财经8月10日讯(记者 畅帅帅)最低工资标准关系到每个人的钱袋子，尤其在疫情期间，更是为低收入人群的基本生活起到“兜底”作用。近期多省份提高失业保险金，而最低工资标准与失业保险金直接“挂钩”。　　据中国网财经记者梳理，截至目前，共有青海、福建以及广西三地宣布上调最低工资标准，北京、上海、天津由于疫情原因，今年不作调整，其他省份暂未公布消息。　　从排行榜来看，上海、北京、广东、天津、江苏、浙江等6省份月最低工资标准(指第一档标准，下同)超过2000元，上海以2480元的标准位列全国榜首。　　桂闽青今年已上调最低工资标准 京津沪暂</t>
+          <t xml:space="preserve">强国社区深入讨论楼主正文显示宽度跟帖显示为跟帖内容主帖显示为
+																											    																													计划预算执行报告里的中国经济：应当有信心
+																(
+															海日旭光
+													08月09日 23:17						)5068字(207/0)
+																											    																													曾写出“最悲伤作文”的凉山小女孩，5年后大变样了
+																(
+		</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>http://slide.news.sina.com.cn/slide_1_86058_474234.html</t>
+          <t>http://bbs1.people.com.cn/board/1.html</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>烛光祈福贝鲁特港口区爆炸伤亡人员</t>
+          <t>强国论坛</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了新闻中心意见反馈留言板新浪简介 | About Sina | 广告服务 | 联系我们 | 招聘信息 | 网站律师 | SINA English | 通行证注册 | 产品答疑Copyright © 1996-2020 SINA Corporation, All Rights Reserved新浪公司 版权所有</t>
+          <t>强国社区强国论坛楼主正文显示宽度跟帖显示为跟帖内容主帖显示为
+																											    																													事关下半年经济工作具体部署 多部委负责人集中发声
+																(
+															今日关注
+													08月10日 08:15						)4930字(753/0)
+																											    																													31省份最低工资：桂闽青已上调 京津沪暂缓调整
+																(</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>http://slide.mil.news.sina.com.cn/c/slide_8_91486_79042.html</t>
+          <t>http://www.chinaql.org/GB/index.html</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>校场：价值连城的阵风战机将如何改变南亚局势</t>
+          <t>中国侨联</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了新闻中心意见反馈留言板新浪简介 | About Sina | 广告服务 | 联系我们 | 招聘信息 | 网站律师 | SINA English | 通行证注册 | 产品答疑Copyright © 1996-2020 SINA Corporation, All Rights Reserved新浪公司 版权所有</t>
+          <t>中国侨联十届五次常委会议举行    7月31日，中国侨联十届五次常委会议召开。会议以电视电话会议的形式举行,主会场设在北京，分会场设在各直辖市、省会（首府）城市和香港、澳门特别行政区。详细+ 听第一书记讲脱贫故事：总书记牵挂老区“脱贫摘帽”     “总书记考察时特意叮嘱我们‘要把富硒品牌做起来’。现在梓山的富硒丝瓜，不仅能卖上好价钱，而且不愁销路。”走进江西省赣州市于都县梓山镇潭头村的蔬菜大棚，翠绿的丝瓜长势喜人，驻村第一书记肖桂花乐呵呵地给记者介绍。详细+ 信息传播部党支部开展“素质提升年”第三次专题党课程学源出席中国侨联青年委员会海外委员代表视频交流座谈会李卓彬副主席对侨创联盟成员提出三</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>https://video.sina.com.cn/p/news/2020-08-10/detail-iivhuipn7765185.d.html</t>
+          <t>http://scitech.people.com.cn/GB/1059/427072/index.html?from=singlemessage&amp;isappinstalled=0</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>新浪资讯台</t>
+          <t>科创</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>正在加载...请稍等~分享视频地址：本页面地址：复制播放器swf地址：复制发布时间：2020-08-10 07:50:55来源：央视频道：新闻中心 / 新闻视频 标签：娱乐明星简介：8月8日，和北京人艺都迎来了疫情后的首场正式售票演出，而以等厂牌为代表的部分单口喜剧已复演约2周。听听北京保利剧院、演员、和单立人喜剧给CGTN讲他们当下的复演情况～</t>
+          <t>9位明星诵读科学家名言向共和国的脊梁致敬[详细]邓中翰：破“缺芯”困局 要占领产业“无人地带”芯片是任何信息发展的核心技术。[详细]徐晓兰：机器换人会助推高质量就业潮产业发展要补短板、布前沿、聚合力、强化合作。[详细]</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>https://video.sina.com.cn/p/news/2020-08-10/detail-iivhuipn7765185.d.html</t>
+          <t>http://yunying.people.cn/GB/index.html</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>北京文化场所复演</t>
+          <t>运营</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>正在加载...请稍等~分享视频地址：本页面地址：复制播放器swf地址：复制发布时间：2020-08-10 07:50:55来源：央视频道：新闻中心 / 新闻视频 标签：娱乐明星简介：8月8日，和北京人艺都迎来了疫情后的首场正式售票演出，而以等厂牌为代表的部分单口喜剧已复演约2周。听听北京保利剧院、演员、和单立人喜剧给CGTN讲他们当下的复演情况～</t>
+          <t xml:space="preserve">      活动在广泛征集参选案例的基础上，通过严格的评审程序产生“入围案例”和“十大杰出案例”。根据参选案例情况，评委会可推荐若干“最佳案例”，旨在激励内容呈现、创意、技术等某方面特别突出，尤其为加强向世界传递中国声音、讲好中国故事贡献力量的“潜力机构”。旗帜网中国互联网发展基金会中文网站红色老区专题中国好人馆全国哲学社会科学工作办公室网站12380举报网党建研究网中国统一战线新闻网周恩来纪念网应急管理部官方微博中国红十字会抖音号国务院扶贫办官方微博中国科学院党建官方微信东方航空微信公众号“MU东东腔”海南岛国际电影节官方微博中国消费者官方微信国新发布APP中国扶贫APP人民网成功承办十七大</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>https://video.sina.com.cn/p/mil/2020-07-20/detail-iivhvpwx6417433.d.html</t>
+          <t>http://dangshi.people.com.cn/GB/151935/427898/index.html</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>军事视频</t>
+          <t>闪光的足迹</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>正在加载...请稍等~分享视频地址：本页面地址：复制播放器swf地址：复制发布时间：2020-07-20 12:34:29来源：新浪军事频道：新浪视频 / 视频新闻 标签：</t>
+          <t xml:space="preserve">    ÎÊ´ð»î¶¯ÔÚ2019Äê9ÔÂ24ÈÕÖÁ10ÔÂ21ÈÕÆÚ¼ä½øÐÐ£¬Ã¿ÖÜÍÆ³ö1ÆÚ£¬¹²4ÆÚ¡£Ã¿ÖÜÒ»ÆÚ´ðÌâ½áÊøºó£¬Ö÷°ì·½´Óµ±ÆÚËùÓÐ´ðÌâÂú·ÖµÄÍøÓÑÖÐËæ»ú³éÈ¡70Î»»ñ½±ÍøÓÑ×÷ÎªÒ»¶þÈýµÈ½±ºÍÐÒÔË½±¡£ÆäÖÐ£ºÒ»µÈ½±1Ãû£¬½±Àø»ªÎªP30ÊÖ»úÒ»²¿£»¶þµÈ½±2Ãû£¬½±Àø»ªÎªÈÙÒ«ÊÖ±íMagicÒ»¿é£»ÈýµÈ½±10Ãû£¬½±Àø¾«ÃÀ¼ÍÄîÆ·Ò»·Ý£»ÐÒÔË½±57Ãû£¬½±Àø¾«ÃÀÎÄ´´²úÆ·Ò</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>https://video.sina.com.cn/p/mil/2020-07-20/detail-iivhvpwx6417433.d.html</t>
+          <t>http://dangshi.people.com.cn/GB/151935/427898/index.html</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>火炮炮口为何会有各种怪“帽子”？视频告诉你</t>
+          <t>我在爱国主义教育基地等你</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>正在加载...请稍等~分享视频地址：本页面地址：复制播放器swf地址：复制发布时间：2020-07-20 12:34:29来源：新浪军事频道：新浪视频 / 视频新闻 标签：</t>
+          <t xml:space="preserve">    ÎÊ´ð»î¶¯ÔÚ2019Äê9ÔÂ24ÈÕÖÁ10ÔÂ21ÈÕÆÚ¼ä½øÐÐ£¬Ã¿ÖÜÍÆ³ö1ÆÚ£¬¹²4ÆÚ¡£Ã¿ÖÜÒ»ÆÚ´ðÌâ½áÊøºó£¬Ö÷°ì·½´Óµ±ÆÚËùÓÐ´ðÌâÂú·ÖµÄÍøÓÑÖÐËæ»ú³éÈ¡70Î»»ñ½±ÍøÓÑ×÷ÎªÒ»¶þÈýµÈ½±ºÍÐÒÔË½±¡£ÆäÖÐ£ºÒ»µÈ½±1Ãû£¬½±Àø»ªÎªP30ÊÖ»úÒ»²¿£»¶þµÈ½±2Ãû£¬½±Àø»ªÎªÈÙÒ«ÊÖ±íMagicÒ»¿é£»ÈýµÈ½±10Ãû£¬½±Àø¾«ÃÀ¼ÍÄîÆ·Ò»·Ý£»ÐÒÔË½±57Ãû£¬½±Àø¾«ÃÀÎÄ´´²úÆ·Ò</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://video.sina.com.cn/p/news/2020-08-10/detail-iivhvpwy0120394.d.html</t>
+          <t>http://finance.people.com.cn/n1/2020/0410/c1004-31668970.html</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>看史诗级救治！首位新冠肺移植出院患者救治过程</t>
+          <t>今年坚决完成贫困人口住房安全有保障目标任务</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>正在加载...请稍等~分享视频地址：本页面地址：复制播放器swf地址：复制发布时间：2020-08-10 00:58:47来源：央视频道：新闻中心 / 新闻视频 标签：健康医疗简介：住院166天，ECMO62天，从死亡线上拉回他，医生说：“感觉人生值得”！，这段震撼视频，为所有医护人员转发，谢谢你们！致敬！</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京4月10日电（许维娜）近日，住房和城乡建设部办公厅印发的《住房和城乡建设部2020年扶贫工作要点》通知指出，坚决完成贫困人口住房安全有保障目标任务，指导和督促各地将“回头看”排查发现的建档立卡贫困户等4类重点对象危房改造任务作为新增任务全部列入2020年中央财政补助资金支持范围，并按照分区分级精准复工复产的要求，有序推动农村危房改造工作。	通知强调，对新增任务较多、排查发现问题突出的地区开展挂牌督战，深入实地开展专项调研督导，确保4类重点对象危房改造扫尾任务于2020年6月底前全部完成。	同时，指导和督促各地对照全国建档立卡贫困户情况，完善</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>http://slide.news.sina.com.cn/slide_1_86058_474235.html</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31817187.html</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>越南高考在疫情下拉开帷幕</t>
+          <t xml:space="preserve">武汉初一初二年级学生返校复学 </t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了新闻中心意见反馈留言板新浪简介 | About Sina | 广告服务 | 联系我们 | 招聘信息 | 网站律师 | SINA English | 通行证注册 | 产品答疑Copyright © 1996-2020 SINA Corporation, All Rights Reserved新浪公司 版权所有</t>
+          <t>登录人民网通行证    立即注册忘记密码？	8月10日，武汉初中阶段初一、初二年级返校复学，至8月30日结束。新华社发（赵军 摄）</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>http://slide.news.sina.com.cn/c/slide_1_86058_474194.html</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31817055.html</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>乡村博物馆里过暑假</t>
+          <t>8月9日强对流天气夜袭北京</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了新闻中心意见反馈留言板新浪简介 | About Sina | 广告服务 | 联系我们 | 招聘信息 | 网站律师 | SINA English | 通行证注册 | 产品答疑Copyright © 1996-2020 SINA Corporation, All Rights Reserved新浪公司 版权所有</t>
+          <t>登录人民网通行证    立即注册忘记密码？	2020年8月9日晚，北京气象台发布18时至23时降水量（毫米）:全市平均17.9，城区平均28.1。大部地区出现7、8级阵风，局地达9到11级。</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>http://slide.news.sina.com.cn/slide_1_86058_474215.html</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31817045.html</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>趣味运动会 快乐度暑假</t>
+          <t>高温下的坚守：铁路编组场里的工务人</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了新闻中心意见反馈留言板新浪简介 | About Sina | 广告服务 | 联系我们 | 招聘信息 | 网站律师 | SINA English | 通行证注册 | 产品答疑Copyright © 1996-2020 SINA Corporation, All Rights Reserved新浪公司 版权所有</t>
+          <t>登录人民网通行证    立即注册忘记密码？	进入8月以来，山城重庆持续高温天气，开启“火炉”模式。位于沙坪坝区的兴隆场编组场，担负着中欧班列（重庆）、陆海新通道、沿江班列的编组任务。8月6日，气温高达39摄氏度,重庆工务段兴隆场线路车间线路巡养三工区，正迎战“高烤”，挥汗如雨,在编组场里进行起道捣固、设备巡检作业。	“我们工区现有16人，主要负责兴隆场编组场三场、四场、七场等共计96.914公里线路，179组道岔的巡检养护。今天主要进行设备巡检、起道捣固、绝缘接头排查整治作业。”工区党员工长谢以见介绍道。此时他正带着工友进行起道捣固作业，确保路线更加平顺。	“捣固机具有六七十斤重，平均每天要捣</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>http://slide.news.sina.com.cn/slide_1_86058_474233.html</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31817080.html</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>疫情下新尝试：泰国“嘟嘟车...</t>
+          <t>河北承德：万寿菊盛放 农民采摘忙</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了新闻中心意见反馈留言板新浪简介 | About Sina | 广告服务 | 联系我们 | 招聘信息 | 网站律师 | SINA English | 通行证注册 | 产品答疑Copyright © 1996-2020 SINA Corporation, All Rights Reserved新浪公司 版权所有</t>
+          <t>登录人民网通行证    立即注册忘记密码？	立秋以来，河北省承德市承德县的种植的万寿菊进入盛花期，当地农民抢抓农时进行第一轮采摘、收储万寿菊工作。	近年来，承德县为推动产业扶贫，采取以“公司+基地+农户”的模式，鼓励当地农户种植万寿菊。万寿菊的花朵是天然叶黄素的主要原料，目前，全县万寿菊种植面积达1.7万亩、参与农户超过5000户，农民通过土地流转和参与打工直接或间接增收致富。刘环宇/人民图片</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/gov/xlxw/2020-08-10/doc-iivhvpwy0150773.shtml</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31817122.html</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>习近平和老乡们说的“贴心话”</t>
+          <t>俄罗斯：丰坦卡河泛轻舟</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：习近平和老乡们说的“贴心话”　　2020年是决胜全面建成小康社会、决战脱贫攻坚之年，也是“十三五”规划收官之年。习近平总书记曾说“扶贫始终是我工作的一个重要内容，我花的精力最多”“我最牵挂的还是困难群众”。　　党的十八大以来，习近平总书记走遍全国14个集中连片特困地区，考察了20多个贫困村。同老乡们在一起，总书记问的是“小事”，算的是细账，谋的是出路，想的是实招，一句句“贴心话”温暖人心。　　央视网《联播+》带您回顾总书记同老乡们说过的“贴心话”，与您一起感受总书记的为民情怀。　　（中央广播电视总台央视网）责任编辑：王树淼 扫描左侧二维码下载，更多精彩内容随你看。（官方微博：新浪新</t>
+          <t>登录人民网通行证    立即注册忘记密码？	俄罗斯圣彼得堡8日举行丰坦卡立式桨板节，人们盛装打扮，划着立式桨板通过圣彼得堡城内河道。 新华社/路透</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/gov/xlxw/2020-08-10/doc-iivhuipn7819291.shtml</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31816870.html</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>习近平勉励第一书记</t>
+          <t>北京：暑期戏水 感受清凉</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：习近平这样勉励第一书记　　“火车跑得快，全靠车头带。”在全面打赢脱贫攻坚的战役中，第一书记是重要力量。党的十八大以来，习近平总书记始终牵挂第一书记，多次勉励第一书记，给他们工作支招。今天，党建网微平台和你一起回顾学习！　　精准选配第一书记　　扶贫开发贵在精准，重在精准，成败之举在于精准。各地都要在扶持对象精准、项目安排精准、资金使用精准、措施到户精准、因村派人（第一书记）精准、脱贫成效精准上想办法、出实招、见真效。　　——2015年6月18日，习近平在贵州召开部分省区市党委主要负责同志座谈会上强调　　在村级层面，要注重选派一批思想好、作风正、能力强的优秀年轻干部和高校毕业生到贫困村</t>
+          <t>登录人民网通行证    立即注册忘记密码？	　　8月9日，市民在南宫五洲植物乐园户外戏水区旁的沙滩上玩沙子。	　　近期，在做好新冠肺炎疫情防控的前提下，位于北京市丰台区的南宫五洲植物乐园户外戏水区对外开放。市民在戏水的同时还可以在沙滩上画沙画、在新游乐项目“丛林网绳”里穿梭跳跃，丰富暑期生活。新华社记者 任超 摄同步：   							恭喜你，发表成功!请牢记你的用户名:，密码:,立即进入个人中心修改密码。30s后自动返回      推荐帖子推荐帖子推荐帖子    推荐帖子推荐帖子推荐帖子!5s后自动返回      推荐帖子推荐帖子推荐帖子    推荐帖子推荐帖子推荐帖子恭喜你，发表成功!5</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/gov/xlxw/2020-08-10/doc-iivhuipn7819296.shtml</t>
+          <t>http://gx.people.com.cn/n2/2020/0810/c179430-34216213.html</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>开展国土绿化 加强地质灾害防治</t>
+          <t>广西：颗粒归仓收粮忙</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：【每日一习话】开展国土绿化行动 加强地质灾害防治　　习近平：开展国土绿化行动，推进荒漠化、石漠化、水土流失综合治理，强化湿地保护和恢复，加强地质灾害防治。　　这段话出自2017年10月18日习近平在中国共产党第十九次全国代表大会上的报告。　　水土保持是国土整治、江河治理的根本，是我国必须长期坚持的一项基本国策。党的十九大以来，我国加快了水土流失综合治理进度，以尊重自然、顺应自然、保护自然的生态文明思想，形成山、水、林、田、湖、草、沙综合治理的新理念，筑起一道道生态安全屏障。　　协同推进山水林田湖草沙综合治理，需要我们牢牢树立保护和改善自然生态环境就是解放和发展生产力的价值观念，摒弃</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网融安8月10日电 近日正值早稻成熟的季节，广西柳州市融安县农民顶高温、冒酷暑，抢抓农时，抢收早稻，确保颗粒归仓。	近年来，融安县狠抓粮食安全，把粮食生产作为首要任务，实施了一系列产业奖补政策，鼓励贫困群众发展产业增收致富，同时还大力推广水稻机械化耕作，全县水稻机收率达80%左右，贫困村已实现整村脱贫，贫困发生率降至1.57%。（张芳 谭凯兴）</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/zx/2020-08-10/doc-iivhvpwy0141806.shtml</t>
+          <t>http://pic.people.com.cn/n1/2020/0810/c1016-31816817.html</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t xml:space="preserve">涉违反国安法 黎智英及两儿子等7人被捕 </t>
+          <t>塞罕坝云雾美如画</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：港媒：涉嫌勾结外国势力，违反香港国安法，黎智英等7人被港警拘捕　　[环球网报道 记者 尹艳辉]香港国安法实施超过1个月，“东网”刚刚消息称，香港警方国安处今（10日）早拘捕乱港分子、“壹传媒”黎智英等7人，涉嫌勾结外国势力，违反香港国安法。　　“东网”引述消息称，黎智英被捕罪名为涉嫌违反国安法中勾结外国或者境外势力危害国家安全罪，另涉及诈骗。消息人士还透露，警方也拘捕其两名儿子，黎见恩及黎耀恩，两人涉嫌勾结外国或者境外势力危害国家安全罪。此外，“壹传媒”也有高层今晨被捕。报道称，身处海外的黎智英助手Mark Simon则被警方通缉。　　另外，香港无线新闻在报道中提到，这是警方第一次</t>
+          <t>登录人民网通行证    立即注册忘记密码？	清晨，位于河北省承德市的塞罕坝国家森林公园云雾缭绕，美景如画。新华社发（刘满仓 摄）</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhuipn7784444.shtml</t>
+          <t>http://zj.people.com.cn/n2/2020/0808/c186327-34213288.html</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>现场曝光 黎智英被锁上手铐带走</t>
+          <t>浙江长兴：晨曦中采菱 丰收中增收</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：香港警方称7人涉危害国家安全被捕 港媒：黎智英被锁上手铐带走　　海外网8月10日电 香港警方在社交媒体上表示，警方今晨（10日）采取拘捕行动，至少7人被捕，全部为本地男子，年龄介乎39岁至72岁。他们涉嫌干犯勾结外国或者境外势力危害国家安全及串谋欺诈等罪。警方行动仍然进行中，不排除更多人被捕。另据香港“东网”报道，香港警方10日早上逮捕了壹传媒创始人黎智英。　　据此前报道，今年7月，香港警方曾向黎智英等人发出传票，要求其到法院应讯，解释其此前不久在铜锣湾参加非法集会一事。连同这张传票，现年72岁的黎智英，已有5宗刑事案件在身，共面对7项控罪。包括“刑事恐吓”、“组织及参与未经批准的</t>
+          <t>日前，在浙江省湖州市长兴县夹浦镇陶家湾村帮扶基地，菱农正迎着晨曦采收新鲜上市的菱角，构成一幅唯美的丰收图景。	浙江省湖州市长兴县夹浦镇陶家湾村帮扶基地的120余亩菱角开始零星上市，低收入与帮扶对象迎来一年中最忙碌最幸福的收获期。等到8月底菱角大批量丰收上市，镇、村将通过党员认购、爱心义卖等方式畅通销售渠道，届时6名低收入农户可实现增收12000元。	近年来，夹浦镇陶通过河道清淤、管网上岸、农村生活污水增点扩面等“水岸同治”举措，大力推进五水共治，水环境和生态环境大大改善，菱角质量和产量大幅提升。（谭云俸、黄可睿、王丽玮）【1】【2】【3】【4】【5】【6】日前，在浙江省湖州市长兴县夹浦镇陶家湾</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhvpwy0171345.shtml</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1024-31817075.html</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>港警：不排除更多人被捕</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1024-31817075.html</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：港警通报：至少7人涉嫌勾结外国或境外势力危害国家安全及串谋欺诈等罪被捕，不排除更多人被捕　　[环球网报道 记者 尹艳辉]香港警方8月10日在官方脸书账号发布消息称，今晨（10日）至少拘捕7名香港男子，他们涉嫌勾结外国或境外势力危害国家安全及串谋欺诈等罪。警方称，拘捕行动仍在进行中，不排除有更多人被捕。　　香港警方在脸书中未提到被捕人士的名字。而在10日稍早，香港“东网”等多家港媒援引消息称，香港警方国安处今 （10日）早拘捕乱港分子、“壹传媒”黎智英、及其两个儿子和多名“壹传媒”高层等7人，涉嫌勾结外国势力，违反香港国安法。　　报道提到，7名被捕人士包括黎智英、其两名儿子黎见恩及黎</t>
+          <t>HTTP ERROR</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhvpwy0175668.shtml</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31816856.html</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>更新服务协议“断供中国”？微软回应</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31816856.html</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　　原标题：微软更新服务协议“断供中国”？微软回应：我们为中国用户提供服务的承诺坚定不移　　[环球时报-环球网报道 记者 范凌志]微软准备断供中国？9日，中文社交媒体上有传言称，微软公司在其官网更新了服务协议，声明如因不可抗力导致微软无法履行或延迟履行其义务，微软对此不承担任何责任或义务。甚至有解读称，微软最近紧急修改了协议，暗示如果美国政府对微软下达禁令，微软可能断供中国，且不提供任何补偿。　　对此，微软公司10日在给环球时报-环球网发来的声明中表示，“近日某些个别社交媒体对微软服务条款全球性更新的谣言，不符合事实。我们为中国用户提供服务的承诺坚定不移”。责任编辑：吴金明 扫描左侧二维码下</t>
+          <t>HTTP ERROR</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-09/doc-iivhvpwy0112605.shtml</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1024-31817250.html</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>因为TikTok 他俩在特朗普面前大吵一架</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1024-31817250.html</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：因为TikTok，他俩在特朗普面前大吵一架　　美国财政部长史蒂文·姆努钦与白宫高级贸易顾问彼得·纳瓦罗。　　不出售便“关门大吉”——这是美国总统特朗普威胁TikTok的套路。然而，对于收购还是封禁TikTok？白宫内部早已出现明显分歧。　　据《华盛顿邮报》8月9日报道，上周末，在白宫椭圆形办公室，美国财政部长史蒂文·姆努钦与白宫高级贸易顾问彼得·纳瓦罗就TikTok相关话题，爆发了一场激烈的争吵。而特朗普就在一边旁观。　　知情人士透露称，当时姆努钦坚持认为，TikTok应出售给一家美国公司。姆努钦曾多次与微软高层进行交谈，他相信自己就微软收购TikTok一事已在白宫内部取得了支持。</t>
+          <t>HTTP ERROR</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/w/2020-08-10/doc-iivhuipn7799112.shtml</t>
+          <t>http://opinion.people.com.cn/n1/2020/0810/c1003-31815900.html</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>盖茨：特朗普杀死脸书唯一竞争对手很奇怪</t>
+          <t>只有中国共产党才能领导中国</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：盖茨谈洽购TikTok：特朗普杀死脸书唯一竞争对手很奇怪　　微软创始人比尔·盖茨将微软对TikTok的并购交易描述为“毒酒圣杯”。　　在8月7日接受Wired采访时，盖茨对微软收购部分TikTok业务明确表示这不会容易，“谁知道这笔交易接下来会发生什么，”盖茨说，“是的，这是个装了毒酒的圣杯。”　　盖茨还指出，要成为社交网络业务的重要玩家“没那么简单”，因为微软将不得不将其内容审查提升到一个全新的水平。　　当问到盖茨是否对微软加入社交媒体的竞争保持警惕时，盖茨表示，让Facebook（脸书）拥有更多竞争对手“可能是件好事”，但“让特朗普杀死唯一的竞争对手，这很奇怪”。　　TheVe</t>
+          <t>登录人民网通行证    立即注册忘记密码？达  仁　　纵览过去百年历史，中华民族由战乱频仍、民不聊生到根本扭转命运、持续走向繁荣富强是一个鲜明标识、主脉主线。引领这一历史大趋势的政治力量，是始终把马克思主义作为行动指南，并坚持在实践中不断丰富和发展马克思主义的中国共产党。　　陈望道在1920年翻译出版的《共产党宣言》，鲜明指出共产党在实际方面是“各国劳动阶级中最进步最果决的一派”，在理论方面“狠能了解劳动运动底进路，情势，以及最后的结果”。从诞生之日起，中国共产党就把实现共产主义作为党的最高理想和最终目标，义无反顾肩负起实现中华民族伟大复兴的历史使命。中国人民发愤图强、艰苦创业，创造了“当惊世</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/w/2020-08-10/doc-iivhuipn7755242.shtml</t>
+          <t>http://rmfp.people.com.cn/n1/2020/0810/c406725-31817092.html</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>美科技巨头头疼</t>
+          <t>52县督战成果丰硕</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：美媒：特朗普禁TikTok让美国科技巨头头疼　　美国彭博社8月8日文章，原题：特朗普禁止TikTok、微信也是美国科技巨头的问题  它终于发生了。在威胁了一个月之后，特朗普总统以国家安全为由，发布行政命令，将禁止在美国受欢迎的中国应用TikTok和微信。　　特朗普的命令对中国应用的威胁显而易见。但命令里所列举的细节，可能也会让美国科技巨头们未来感到头疼。例如，特朗普称，TikTok收集位置数据和用户活动信息，这些信息“可能”被用于勒索和商业间谍活动。这一说法也适用于所有美国的社交媒体应用。问题是，这种说辞为其他国家使用类似理由禁止美国应用打开了大门。经过这么长时间的调查，针对这些应</t>
+          <t>登录人民网通行证    立即注册忘记密码？	国务院扶贫办副主任欧青平（图片来源：国新网徐想 摄）	人民网北京8月10日电（记者 勾雅文 史雅乔）8月10日下午3时，国务院新闻办公室举行新闻发布会，介绍挂牌督战工作成果情况，并答记者问。	国务院扶贫办副主任欧青平在发布会上介绍挂牌督战工作有关背景和进展情况时表示，经过半年时间的努力，挂牌督战地区的脱贫攻坚工作进展非常顺利，脱贫攻坚专项巡视回头看、成效考核等发现的各类问题整改也基本完成。	据欧青平介绍，52个挂牌县三保障和饮水安全的存量问题都已经全部解决，易地扶贫搬迁剩余的任务全部完成，今年挂牌地区贫困劳动力外出务工规模已超过了去年，就业保持了基本</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-09/doc-iivhuipn7736529.shtml</t>
+          <t xml:space="preserve">http://rmfp.people.com.cn/n1/2020/0810/c406725-31817160.html </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>美国卫生部长抵台 洪秀柱开炮了！</t>
+          <t>医保全覆盖</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：美国卫生部长抵台，洪秀柱开炮了！　　洪秀柱质问台当局：他来台湾能做什么？　　“阿扎来台无需隔离入境的目的到底是什么？他来台湾能做什么？政府这都无法说清楚，如何让人支持？”美国卫生部长阿扎今天（9日）访台，却不需要隔离14日，国民党前主席洪秀柱怒抛3问质问民进党当局。　　据台湾“联合新闻网”“中时电子报”等台媒报道，美国卫生部长阿扎今天（9日）访台，却不需要隔离14日，遭岛内民众质疑这是特权，岛内民众还担心恐成防疫漏洞。国民党前主席洪秀柱今天（9日）怒抛3问质问民进党当局：美国现在是全世界确诊人数最高的国家，在这么严峻的情势下，阿扎来台无需隔离入境的目的到底是什么？他来台湾能做什么？</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电（记者 史雅乔 勾雅文）8月10日下午3时，国务院新闻办公室举行新闻发布会，介绍挂牌督战工作成果情况，并答记者问。	国务院扶贫办副主任欧青平在回答记者提问时表示，保障贫困人口的基本医疗是脱贫的重要标准“三保障”之一，目前，全国累计有1800多万贫困患者得到了有效救治，一共有1007家各地的三级医院与1172家贫困县的医院开展了结对帮扶。从医疗有保障这个角度来讲，所有的贫困人口都已经纳入了基本医疗保险的范围。	据欧青平介绍，脱贫攻坚以来，国家卫生健康委、国家医保局等相关部门认真贯彻中央关于健康扶贫工作的部署，出台了一系列面向贫困地</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhvpwy0204455.shtml</t>
+          <t xml:space="preserve">http://rmfp.people.com.cn/n1/2020/0810/c406725-31817130.html </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>多少印度人认为印度军力比中国强？结果有点震撼</t>
+          <t>保持督促力度</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：多少印度人认为印度军力比中国强？结果有点震撼　　如果中国和印度因边界争端走向战争会发生什么？印度卡维洞察（Karvy Insights)）“国家情绪调查”（MOTN）显示，72%的印度人自信地认为印度军队能战胜中国的军队。　　该调查的提出的问题是：“你认为印度的军事能力和中国相比如何？” 72%的印度人民认为印度能在和中国的对抗中获胜；9%的印度人民回应“我们不能打赢中国”；10%的人认为两国最后会陷入僵局；还有9%没有发表意见。　　这一调查是在今年的7月15日至27日进行的，共有12021名受访者回复了这一调查问卷，其中67%来自农村区域，33%来自城市。　　此外，在该机构其它关</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电（记者 勾雅文 史雅乔）8月10日下午3时，国务院新闻办公室举行新闻发布会，介绍挂牌督战工作成果情况，并答记者问。国务院扶贫办副主任欧青平在答记者问时表示，脱贫攻坚的任务并没有全面完成，下一步将督促指导各地重点推进三个方面的重点工作。	一是继续抓好“三保障”和饮水安全的查漏补缺。虽然所有尚未存量问题已经解决，但还有一些新增的住房不安全问题和饮水不安全问题存在，这些问题要及时发现、及时地解决。	二是多措并举，促进稳岗就业。上半年解决了贫困劳动力“出的去”问题，把贫困劳动力送出去，下半年就是怎么把贫困劳动力稳在就业的当地，稳在就业的</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-09/doc-iivhvpwy0099634.shtml</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31817220.html</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>在京开会后公安部部长赴东北：决不允许搞“伪忠诚”</t>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31817220.html</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：在京开会后，公安部部长赴东北：决不允许搞“伪忠诚”！　　来源：北京青年报　　撰文 |  余晖　　8月6日至8日，国务委员、公安部党委书记、部长赵克志在吉林和黑龙江调研了3天，公安部副部长杜航伟陪同。　　这是赵克志在京召开全国公安机关“坚持政治建警全面从严治警”教育整顿动员部署会议后，首次离京。　　了解民警工资收入、调研教育整顿　　据公安部官网披露，赵克志在东北行程包括：　　其一，到吉林、黑龙江的省市县三级公安机关和基层派出所，慰问公安民警辅警　　其二，他就开展“坚持政治建警全面从严治警”教育整顿、全力做好当前维护安全稳定工作进行了调研　　报道中提到，每到基层所队，赵克志都与执勤民警</t>
+          <t>HTTP ERROR</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/zx/2020-08-10/doc-iivhuipn7764270.shtml</t>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816711.html</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>中美将重新评估贸易协议？驻美大使回应</t>
+          <t>7月份CPI同比上涨2.7%</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：崔天凯：中美关系处于非常关键时刻，今天的抉择将塑造世界的未来　　8月4日，崔天凯大使应邀出席2020年阿斯彭安全论坛，就中美关系有关问题与阿斯彭战略小组执行主任尼古拉斯·伯恩斯以及美国全国广播公司对外政策首席记者安德利亚·米歇尔进行在线对话，并回答观众提问。全文实录如下：　　伯恩斯：崔大使，谨向您致以最热烈的欢迎。在把采访转交给安德利亚·米歇尔之前，我想阐述一点想法。我认为美中关系可能处于1971年、1972年尼克松总统打开中国大门以来的最低点。在美国，人们对中国政府放弃其对香港人民的承诺、印度与中国在喜马拉雅山地区发生边界冲突，以及中国在南海的活动感到非常关切。几十年以来，你和我</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 （杨曦）国家统计局今日公布数据显示，2020年7月份，全国居民消费价格（CPI）同比上涨2.7%，环比上涨0.6%。1―7月，全国居民消费价格比去年同期上涨3.7%。	从同比看，城市上涨2.4%，农村上涨3.7%；食品价格上涨13.2%，非食品价格持平；消费品价格上涨4.3%，服务价格持平。	从环比看，城市上涨0.6%，农村上涨0.8%；食品价格上涨2.8%，非食品价格持平；消费品价格上涨1.0%，服务价格下降0.1%。	国家统计局城市司高级统计师董莉娟表示，7月份，各地区各部门统筹做好疫情防控、抢险救灾和经济社会发展工作，积</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhuipn7791977.shtml</t>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816704.html</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>美国希望中国打第一枪？专家：千万不能中了它的计！</t>
+          <t>PPI降幅收窄</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：美国希望中国打第一枪？专家：千万不能中了它的计！　　张彬表示，目前在两岸局势紧张的情况下，美国是希望大陆打出第一枪的，我们一定不能上当，要保持战略定力，不能随美国起舞。而还在炒作大陆演习的“台独”分子只看到目前所得到的好处，却不知道中国沿海的任何动荡，台湾都不可能独善其身。责任编辑：吴金明 扫描左侧二维码下载，更多精彩内容随你看。（官方微博：新浪新闻）违法和不良信息举报电话：4000520066                    举报邮箱：jubao@vip.sina.comCopyright © 1996-2020 SINA CorporationAll Rights Res</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 （杨曦）国家统计局今日公布数据显示，2020年7月份，全国工业生产者出厂价格（PPI）同比下降2.4%，降幅比上月收窄0.6个百分点。从环比看，PPI上涨0.4%，涨幅与上月相同。	工业生产者购进价格同比下降3.3%，环比上涨0.9%。1至7月平均，工业生产者出厂价格比去年同期下降2.0%，工业生产者购进价格下降2.7%。工业生产者价格同比变动情况	工业生产者出厂价格中，生产资料价格同比下降3.5%，降幅比上月收窄0.7个百分点，影响工业生产者出厂价格总水平下降约2.56个百分点。其中，采掘工业价格下降7.1%，原材料工业价格</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/w/2020-08-10/doc-iivhvpwy0177229.shtml</t>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816775.html</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>特朗普又吹嘘政绩 被当场戳穿后一言不发负气离场</t>
+          <t>解读</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：特朗普又在记者会上吹嘘政绩，被当场戳穿后一言不发负气离场　　美国总统特朗普曾多次声称自己签署了《退伍军人选择法》，并以此作为任期内的政绩。在当地时间8月8日举行的新闻发布会上，特朗普强调他签署了该法案，不料被一名记者当面戳穿谎言，他未做任何解释，立即结束了发布会离开现场。　　据美国有线电视新闻网（CNN）报道，特朗普8日在新泽西州贝德明斯特的高尔夫俱乐部举行新闻发布会，他在会上再次声称自己签署了《退伍军人选择法》，“数十年来，他们一直寻求让法案通过，但是没有一个总统做到，而我们做到了。“　　随后，哥伦比亚广播公司（CBS）记者保拉·瑞德当场质问总统：“为什么你一直说自己通过了《退伍</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 （杨曦）国家统计局今天发布了2020年7月份全国CPI（居民消费价格指数）和PPI（工业生产者出厂价格指数）数据。对此，国家统计局城市司高级统计师董莉娟进行了解读。CPI环比由降转涨，同比涨幅略有扩大	7月份，各地区各部门统筹做好疫情防控、抢险救灾和经济社会发展工作，积极落实保供稳价政策，市场运行总体有序。从环比看，CPI由上月下降0.1%转为上涨0.6%。其中，食品价格上涨2.8%，涨幅比上月扩大2.6个百分点，影响CPI上涨约0.62个百分点。食品中，随着餐饮服务等逐步恢复，猪肉消费需求持续增加，而多地洪涝灾害对生猪调运产</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhuipn7802170.shtml</t>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31816950.html</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>林夕更改《约定》歌词支持罗冠聪 网友:眼盲心更盲</t>
+          <t>幸福花开新边疆:鄂温克太阳姑娘</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：林夕更改《约定》歌词支持罗冠聪，香港网友：眼盲心更盲　　近日，正在被通缉的“乱港分子”头目罗冠聪多次在社交媒体上宣称自己“人在英国，心系香港”，这一虚伪说法居然还得到了香港作词人林夕的回应，7日，林夕在个人社交媒体上写下“还记得当天抗争多难捱”、“仍未忘跟你约定心念没有死”等，文末带上了罗冠聪的话题，并配图“约定”。　　《约定》原是由林夕填词，王菲演唱的一首歌，林夕在帖子中将歌词做了修改。　　林夕，香港知名文字工作者，尤以填词人及多媒体创作人身份为人熟悉，是香港乐坛创作作品最多的填词人之一。2008年北京奥运会的《北京欢迎你》就是出自他手，但他后来竟称为奥运歌曲填词是“人生污点”，</t>
+          <t>登录人民网通行证    立即注册忘记密码？	　　央视网消息（记者 董淑云 王若怡 邢明）：八月的呼伦贝尔大草原，苍茫辽阔，与天相接。一场微雨过后，芳草的清香在湿润的空气中弥漫开来，沁人心脾。牛羊悠闲地低头啃草，安逸而宁静。	　　在内蒙古自治区东北部的呼伦贝尔市鄂温克族自治旗，乌仁与“太阳姑娘”家喻户晓。乌仁不仅是民族手工艺品制作能人，还是当地妇女致富的带头人。	　　乌仁与记者分享她的创业故事	　　“太阳花”点亮新生活	　　在鄂温克族的传统饰品中，用牛羊的皮毛等制作的“太阳花”是常用的装饰品，皮质的圆心象征太阳，四周的毛针如同阳光一般，乌仁说：“这代表我们鄂温克族对温暖和光明的向往。”	　　乌仁</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/w/2020-08-10/doc-iivhuipn7828556.shtml</t>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31816956.html</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>美总统大选临近 中俄在美国展开激烈较量？</t>
+          <t xml:space="preserve"> 义勒力特风景</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：中俄在美国展开激烈较量？　　随着美国2020年的总统大选还有不到3个月就将来临，美国现任共和党籍总统特朗普，以及他的挑战者、曾担任过美国副总统的民主党籍政客拜登，都在拼命攻讦和抹黑对方，以求瓦解对手的政治形象。　　而随着这种政治互撕变得越发的“歇斯底里”，双方甚至连常识和逻辑都不顾了，并由此诞生了我们今天要和大家说的一个令人捧腹的大笑话。　　首先，我们都知道特朗普为了赢得此次总统大选而采取的一个最主要的竞选策略，就是拼命攻击中国，比如将新冠病毒说成是“中国病毒”，并将由他的工作失职所导致的美国疫情大失控说成是中国“害的”，来将美国国内的矛盾和不满转移到一个“外国势力”上。　　而他对</t>
+          <t>登录人民网通行证    立即注册忘记密码？	　　这个季节，站在敖包山顶，一眼望去，稻浪如海，“红城1947”、“兴安盟大米 内蒙古味稻”两幅巨大的3D彩稻景观画栩栩如生。走在小镇的路上，鲜花随处可见，绿树成荫，流水清澈，特色民宿、孔雀园、开心农场等吸引很多游客前来。这是位于内蒙古兴安盟乌兰浩特市的义勒力特小镇，它是远近闻名的“花香小镇”。	图为义勒力特镇的稻田画。（经济日报-中国经济网记者 武晓娟/摄）	　　近年来，义勒力特镇凭借自身生态优势，借力“全域旅游”，逐步深化“旅游+”的创新理念，以增加百姓收入、鼓起农民腰包为落脚点，大力发展优势产业和特色产业，带动地方经济发展。	　　图为义勒力特镇</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhuipn7828301.shtml</t>
+          <t>http://hm.people.com.cn/n1/2020/0810/c42272-31815902.html</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>港媒警告：台湾勿以为11月3日前是安全期</t>
+          <t>国务院港澳办</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：港媒警告：台湾勿以为11月3日前是安全期　　台湾现在最可怕的是，区域波涛汹涌，但台湾人在刻意营造出来的歌舞升平气氛下，毫无危机意识！　　香港中评社刊载评论员林淑玲撰写的社评说，美国卫生与公众服务部部长阿扎率领的代表团9日下午搭专机抵达松山机场，吊唁李登辉，拜会蔡英文，预计停留到12日。美国的大动作，再度挑动了美中关系和两岸关系。台湾若有11月3日美国大选前是安全期的想法，将是一项极危险的认知。　　美国正在把台湾推上火线　　距离美国大选只剩下2个多月，若以目前民调，美国总统特朗普要赢得连任，几乎不可能。因此在过去的10多天，美国猛烈加大挑战北京动作，封杀抖音后，又锁定腾讯，指派卫生部</t>
+          <t>登录人民网通行证    立即注册忘记密码？　　新华社北京8月9日电  国务院港澳事务办公室发言人9日发表谈话表示，美国当局近日宣称对中国政府涉港部门负责人和香港特别行政区政府有关官员实施制裁，充分暴露出美国一些政客的霸权主义习性，是其在香港问题上的政治盘算失算后的一次歇斯底里式的发作，也注定是徒劳的。　　发言人表示，去年6月香港“修例风波”发生以来，美国一些反华反共势力以为找到了策动“颜色革命”的新机会，频密安排香港反对派头面人物访问美国并高规格接待，公开为街头暴力活动鼓噪叫好，大肆抹黑攻击特区政府和警方的执法行动，并通过各种方式为香港反对派和激进势力提供支持，为他们撑腰打气。他们还对香港反对</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-09/doc-iivhvpwy0093710.shtml</t>
+          <t>http://hm.people.com.cn/n1/2020/0810/c42272-31815904.html</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>一度被称“花花公子热” 上海已现9例威胁39亿人</t>
+          <t>香港中联办批驳美国所谓制裁</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：一度被称为“花花公子热”，上海已出现9例，威胁全球39亿人……　　来源：瞭望智库　　文 | 张文宏 上海华山医院感染科主任　　最近，登革热进入高发季节，世界多地都发现病例。　　8月3日，厦门发布登革热高风险等级。截至8月7日，据上海市疾控中心消息，上海市已报告输入性登革热病例9例。　　而在新加坡，截至4日，每周新增登革热病例连续8周超过1000例，今年已出现22403例登革热病例，超过2013年全年22170例的历史最高纪录。截至8月2日，新加坡因感染登革热病毒死亡人数已达20人。　　有数据显示，全球每年大约有3.9亿例登革热感染病例，出现临床症状的病例数大约为9600万。另一项研</t>
+          <t>登录人民网通行证    立即注册忘记密码？	　　本报香港8月9日电  （记者冯学知）中央人民政府驻香港特别行政区联络办公室发言人9日发表谈话指出，近日香港舆论场形成谴责美霸权主义行径的强劲声浪，中方有关表态得到舆论和网民的喝彩。公道自在人心，主流民意再次证明美方所谓制裁蛮横无理，最终只会沦为全世界笑柄。	　　发言人表示，从昨天到现在，中央有关涉港工作部门、特区政府先后作出公开回应，表达了强烈谴责美恶劣行径的严正立场。被美列入制裁名单的我方官员公开表态“无惧美国制裁”，体现了对国家和香港利益的坚定捍卫和忠诚担当。这些回应被香港媒体广泛报道，社会各界纷纷发声支持呼应，相关内容在网上持续产生刷屏效应</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/c/2020-08-10/doc-iivhuipn7762934.shtml</t>
+          <t>http://world.people.com.cn/n1/2020/0810/c1002-31815896.html</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>烧了66亿元卖了31辆 车企董事长称“没有任何责任”</t>
+          <t>美学者:用"新冷战"概念看待美中关系有误导性</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：江苏赛麟造车大败局：烧了66亿元卖了31辆，董事长称“没有任何责任”　　百日之内，耗时四年造车的赛麟汽车“猝死”　　身处美国的王晓麟和如皋政府隔空对峙，互相指责　　导致公司停摆的原因在于对方　　江苏赛麟造车大败局　　本刊记者／苏杰德  胥大伟　　发于2020.8.10总第959期《中国新闻周刊》　　赛麟汽车“骗局”被捅破，已经逾百日。　　今年4月27日，江苏赛麟汽车前高级法务经理乔宇东实名举报公司董事长、CEO兼法定代表人王晓麟，对王晓麟涉嫌虚假技术出资及挪用巨额国资提出质疑。　　乔宇东的指控描述了一个“空手套白狼的国际骗局”：王晓麟实际控制的赛麟公司的4个外资企业股东，以虚假技术</t>
+          <t>登录人民网通行证    立即注册忘记密码？	　　本报华盛顿8月9日电  （记者胡泽曦）日前，美国哈佛大学教授、国防部前助理部长约瑟夫・奈通过电子邮件对本报记者表示，美国国务卿蓬佩奥不久前在尼克松总统图书馆暨博物馆就对华政策发表的演讲，主要反映了美国大选年国内政治对外交政策的影响。他强调，用“新冷战”概念看待美中关系具有误导性。	　　约瑟夫・奈在邮件中指出，当前美国和中国之间的相互依赖程度非常高。美中之间确实存在问题和分歧，但过去两国就曾做到妥善管理彼此间的问题和分歧。当前应对新冠肺炎疫情全球大流行，需要美中进行合作。约瑟夫・奈还表示，他本人不希望看到美国民众受政治人物影响，转而支持一种类似冷战</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/zx/2020-08-10/doc-iivhvpwy0196619.shtml</t>
+          <t>http://world.people.com.cn/n1/2020/0810/c1002-31815895.html</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>四川一女子一家五口被杀：前男友有重大嫌疑 已坠亡</t>
+          <t>多国媒体高度评价北斗三号导航系统开通</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：警方通报四川一家五口被杀：犯罪嫌疑人已坠楼身亡责任编辑：张建利 扫描左侧二维码下载，更多精彩内容随你看。（官方微博：新浪新闻）违法和不良信息举报电话：4000520066                    举报邮箱：jubao@vip.sina.comCopyright © 1996-2020 SINA CorporationAll Rights Reserved  新浪公司 版权所有 </t>
+          <t xml:space="preserve">登录人民网通行证    立即注册忘记密码？	　　北斗三号全球卫星导航系统日前正式开通，中国成为世界上第三个独立拥有全球卫星导航系统的国家。外国媒体对此高度关注，认为中国建成了独立自主、开放兼容的全球卫星导航系统，是中国对世界的重要贡献，不仅可为全球公共服务基础设施建设提供高质量服务，而且对推动全球经济社会发展也将发挥积极作用。	　　北斗系统卫星新技术占比超过70%――北斗卫星导航系统的研发之路，是一条自主创新、追求卓越的发展道路。马来西亚《星报》网站在报道中引述专家评价，认为北斗三号全球卫星导航系统全面建成并开通服务，是中国航天领域新的里程碑，也是中国促进科学技术创新发展的一项重大成就。	　　</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/s/2020-08-10/doc-iivhuipn7790941.shtml</t>
+          <t>http://opinion.people.com.cn/n1/2020/0810/c1003-31815907.html</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>河北12岁女孩遭绑架杀害 警方通报案件细节</t>
+          <t>评</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：任丘市公安局警情续报　　8月10日，河北任丘公安官方微信发布警情通报：8月4日，任丘市麻家务镇北畅支二村发生一起绑架杀人案。8月8日6时许公安机关将犯罪嫌疑人宋某某、张某某一举抓获，并缴获涉案赃款100万元。　　案件发生后，公安机关立即成立专案组，迅速展开现场勘查、调查走访、排查搜寻、查缉布控等工作。　　经查，犯罪嫌疑人宋某某、张某某（女）认为受害人家中经济条件较好，遂合谋绑架勒索钱财。8月4日，两名犯罪嫌疑人将受害人赵某某控制后致其死亡，并向其家人索要100万元赎金。8月5日2时许，犯罪嫌疑人将赎金取走并藏匿。　　经讯问，两名犯罪嫌疑人对犯罪事实供认不讳，公安机关已对其依法采取刑</t>
+          <t>登录人民网通行证    立即注册忘记密码？余建斌　　“复移小凳扶窗立，教识中天北斗星。”自古以来，北斗七星就被赋予了司南功能，用以指引方向、分辨四季、标定时刻，中国人对北斗有着熟悉而亲切的认知。如今，仰望星空，由数十颗人造卫星组成的新的北斗“星座”更加璀璨。　　7月31日，习近平总书记在北京人民大会堂郑重宣布，北斗三号全球卫星导航系统正式开通。由我国建成的独立自主、开放兼容的卫星导航系统，从此走向了服务全球、造福人类的时代舞台。这是自豪的宣告，折射出这一完全自主建设、独立运行的巨型复杂航天系统的来之不易；这也是热情的邀约，体现了中国北斗作为向全世界贡献的重大公共服务基础设施，致力于为全球提供导</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/w/2020-08-10/doc-iivhvpwy0154040.shtml</t>
+          <t>http://military.people.com.cn/n1/2020/0810/c1011-31816740.html</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>特朗普想把自己脸刻上“总统山” 网友满足他(图)</t>
+          <t>俄测试新型核潜艇有何战略作用?</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：特朗普想上总统山，网友满足他　　【文/观察者网 徐蕾】好大喜功的特朗普最近被曝出，想把自己的脸也刻在“总统山”上，与乔治·华盛顿、托马斯·杰斐逊、西奥多·罗斯福和亚伯拉罕·林肯并列。　　这座山是美国南达科他州的拉什莫尔山，尽管美国国家公园管理局表示，考虑到安全问题，“总统山”上已经不可能再“加脸”了，但是推特网友早就安耐不住，想帮特朗普实现愿望了。　　一次性来四个，“加脸”加个够！　　有人觉得特朗普可能更想和他的朋友们待在一起：左起分别是比尔·考斯比、韦恩斯坦、爱泼斯坦，三人均被指控性侵。　　还有各式各样的：　　听到特朗普也想“上山”，4位前总统的内心是崩溃的……　　其实，这并不是</t>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电（黄子娟、莫仕伟）据俄罗斯卫星网8月1日报道，俄罗斯国防部宣布，开始测试“别尔哥罗德”号核潜艇，它将成为首个装配有核动力“波塞冬”无人潜艇的载体。相关数据表明，“波塞冬”弹头的功率相当于两百万吨TNT。这种特殊弹药足以摧毁大型沿海城市，海军基地并造成核海啸。	如何看待无人潜艇的作用？它与传统的潜艇武器有何区别？一旦“别尔哥罗德”号正式服役，它将发挥怎样的战略作用？该型潜艇的出现，会让俄罗斯海军武器装备发展重新“洗牌”吗？针对上述问题，人民网专访军事专家尹卓，他认为，该型潜艇的研发有助于俄罗斯培育战略上的非对称优势。战略上的非对称</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://finance.sina.com.cn/roll/2020-08-10/doc-iivhuipn7849913.shtml</t>
+          <t>http://sports.people.com.cn/n1/2016/0722/c14820-28575143.html</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>央行：办理花呗业务小贷公司拟恢复报送信贷业务信息</t>
+          <t>［阅读］</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：央行：办理“花呗”业务的小额贷款公司拟于近期恢复报送信贷业务信息 　　中证网讯（记者 彭扬）央行有关部门负责人日前对中国证券报记者表示，办理“花呗”业务的小额贷款公司于2015年4月接入征信系统，后因放贷主体发生变更暂停报送信贷业务信息，拟于近期恢复报送。办理“京东白条”业务的小额贷款公司于2019年5月接入征信系统，相关业务信息报送情况良好。　　上述负责人介绍，按照《征信业管理条例》第二十八条规定：“金融信用信息基础数据库接收从事信贷业务的机构按照规定提供的信贷信息。”第二十九条规定：“从事信贷业务的机构应当按照规定向金融信用信息基础数据库提供信贷信息”。“花呗”和“京东白条”信</t>
+          <t>登录人民网通行证    立即注册忘记密码？本报记者  刘  �i					 	　　从1900年首度进入奥运殿堂，到1908年成为奥运正式项目，帆船项目已经是奥运历史上的老面孔。尽管中国开展帆船运动的时间不长，但越来越多的人正在参与并爱上这项“中流击水、浪遏飞舟”的运动。尤其是自2008年收获首枚奥运金牌以来，帆船热正在席卷中国各大沿海城市。	　　近日，随着中国奥运代表团成立，中国帆船队征战里约奥运的运动员名单也随之出炉。此次里约奥运，中国将有8名帆船选手出战。	　　徐莉佳迎复出战	　　奥运阵容中，徐莉佳无疑是最具夺金希望的一人。2008年，在青岛举行的奥运会帆船比赛，徐莉佳获得一枚宝贵的铜牌。</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://video.sina.com.cn/p/news/2020-08-10/detail-iivhuipn7758139.d.html</t>
+          <t>http://leaders.people.com.cn/n1/2020/0810/c178291-31816988.html</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>北京确定秋季学期开学时间</t>
+          <t>7月网上群众工作数据报告</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>正在加载...请稍等~分享视频地址：本页面地址：复制播放器swf地址：复制发布时间：2020-08-10 06:36:23来源：央视频道：新闻中心 / 新闻视频 标签：朝闻天下</t>
+          <t>登录人民网通行证    立即注册忘记密码？	相关阅读：2020上半年各级干部通过人民网《领导留言板》回应群众建言与诉求27万余件5月份网民给各级领导干部留言近7万件 有5.1万件获答复4月份网民给各级领导干部留言7.3万件 有5.6万件获答复3月份各级领导干部回应留言4.6万件 复工复产难题受关注2月份各级领导干部回应留言超3万件 同比增长近80%1月网民给各级领导干部留言4.5万件 有3.5万件获答复微信微博手机人民网领导留言板探访解放碑夜市暴雨后村民齐捞鱼微视频《守护》丈夫雨中撑伞护妻</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>http://slide.news.sina.com.cn/slide_1_91107_428213.html</t>
+          <t>http://nm.people.com.cn/n2/2020/0810/c196689-34216451.html</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>北朝墓葬壁画上的现实与异想世界</t>
+          <t>呼和浩特：打造筑巢引凤新格局</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>已收藏!您可通过新浪首页(www.sina.com.cn)顶部 “我的收藏”， 查看所有收藏过的文章。知道了</t>
+          <t>登录人民网通行证    立即注册忘记密码？富丽娟恳谈会现场。陈立庚 摄	“我们相信，良好的营商环境就像水草丰美的草原，只有草原丰美，'骏马'才会结队而来；我们深知，服务比优惠更关键、诚信比承诺更重要，将全力以赴为企业发展提供全周期、最便利的服务。”8月9日上午，“美丽青城 草原都市”呼和浩特（青岛）企业家恳谈会在青岛国际会议中心召开，内蒙古自治区党委常委、呼和浩特市委书记王莉霞在作推介致辞时表示。	来自山东省的近300家企业负责人参加恳谈，寻找商机、合作共赢，牵手草原共谋发展大计，敖包相会同创精彩未来。内蒙古自治区党委常委、呼和浩特市委书记王莉霞向青岛推介塞外青城。陈立庚 摄	王莉霞指出，要为</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/</t>
+          <t>http://www.people.com.cn/</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://news.sina.com.cn/gov/2020-08-10/doc-iivhvpwy0171573.shtml</t>
+          <t>http://cq.people.com.cn/n2/2020/0810/c365401-34216610.html</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>31省份最低工资：这三省已上调</t>
+          <t>脱贫路上不让一个残疾人掉队</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t xml:space="preserve">　　原标题：31省份最低工资：桂闽青已上调 京津沪暂缓调整　　中国网财经8月10日讯(记者 畅帅帅)最低工资标准关系到每个人的钱袋子，尤其在疫情期间，更是为低收入人群的基本生活起到“兜底”作用。近期多省份提高失业保险金，而最低工资标准与失业保险金直接“挂钩”。　　据中国网财经记者梳理，截至目前，共有青海、福建以及广西三地宣布上调最低工资标准，北京、上海、天津由于疫情原因，今年不作调整，其他省份暂未公布消息。　　从排行榜来看，上海、北京、广东、天津、江苏、浙江等6省份月最低工资标准(指第一档标准，下同)超过2000元，上海以2480元的标准位列全国榜首。　　桂闽青今年已上调最低工资标准 京津沪暂</t>
+          <t>登录人民网通行证    立即注册忘记密码？胡虹 实习生何雨霁	唐文彬正在剥苞米，为家禽准备食物。何雨霁摄	　　在重庆市大足区中敖镇洪溪村，从崖上沿S型土路往下走，崖半腰就是唐文彬的家。四间砖混房建在一处缓坡上，走下一列石阶，就看到唐文彬。	　　他端着个塑料盆，佝偻起身子，一拐一拐地走进屋子旁边的矮小鸡舍。尽管腿脚有些不便，但每一步他都走得精气神十足。鸡舍由木条和铁丝网围成，里面有十来只鸡。他从盆子里抓一把黄澄澄的苞米粒儿，嘴里一边吆喝着“咯咯咯”，一边往地面一撒。鸡群很快凑拢过来，争先恐后地啄食。	　　“把鸡养大，可以卖个好价钱，还可以下蛋来吃。”唐文彬心中美滋滋的盘算着。前段时间，他刚卖出了</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>http://travel.people.com.cn/n1/2020/0810/c41570-31816987.html</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>重游湖北,他们说:"这里很安全!"</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿	8ÔÂ8ºÅÆð£¬ºþ±±Ê¡ËùÓÐA¼¶ÂÃÓÎ¾°Çø¶ÔÈ«¹úÓÎ¿ÍÃâÃÅÆ±¿ª·Å¡£ÖÜÄ©Á½Ìì£¬Îäºº»Æº×Â¥¡¢ÏåÑô¹ÅÂ¡ÖÐ¡¢¾£ÖÝ¹Å³Ç¡¢Ê®ÑßÎäµ±É½µÈÖøÃû¾°ÇøÈËÆø±¬Åï¡£ÆäÖÐ£¬ÓÐÒ»ÅúÌØÊâµÄ¿ÍÈË£¬À´×Ô23¸öÊ¡·ÝµÄ72ÃûÔ®¶õÒ½ÁÆ¶ÓÔ±±¸ÊÜ¹Ø×¢£¬¸ÐÊÜ¾£³þ´óµØÒßºóÖØÉúµÄ²ª²ªÉú»ú¡£	Ô®¶õÒ½ÁÆ¶Ó¶ÓÔ±ÔÚ¹ÅÂ¡ÖÐºÏÓ°	Ô®¶õÒ½ÁÆ¶Ó</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>http://media.people.com.cn/n1/2020/0810/c120837-31816431.html</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>网络直播深入整治更严更细</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？人民网记者 赵光霞 宋心蕊	8月3日，国家网信办等8部门联合召开工作部署会，通报自6月5日启动的网络直播行业专项整治和规范管理行动的阶段性成果。2个月来，各部门依法处置158款违法违规直播平台，挂牌督办38起涉直播重点案件，并封禁一批违法违规网络主播。	中国传媒大学人类命运共同体研究院副院长王四新在接受人民网记者采访时，对专项整治行动取得的阶段性成果发表了自己的看法：“专项行动整体上改善了直播行业的不良风气，也对网络直播领域的内容生态向好发展起到了推动作用。”	为进一步遏制行业乱象，营造健康向上的网络直播空间，此次会议也对深入推进专项整治和规范管理工作</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31815939.html</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>岗位稳，企业有后劲</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？本报记者  姚雪青　　开栏的话　　疫情防控期间，很多企业压力不小：产品需求受到影响，员工就业还得保障。不少企业迎难而上，在政府的帮扶下，和员工携手共渡难关，兼顾了保就业和保发展。保市场主体就是保民生，同时，岗位稳定，企业发展更有后劲。这些故事值得书写。本版今起推出“就业故事・携手渡难关”系列报道，敬请关注。　　　　宽阔的江面中，各地运货船来来往往；岸边的码头上，装卸车进出不停；港口的堆场里，不同货种码放有序……在江阴，一家港口集团的码头一片繁忙景象，平均每天的吞吐量达到20万吨。眼前的场景表明，目前港口物流业运行平顺、上下游产业发展良好。　　看着半年度</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/n1/2020/0810/c1003-31815919.html</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>抢抓农时 恢复生产</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？臧春蕾　　暴雨肆虐过的农田里，机器轰鸣、村民劳作，一派繁忙。各受灾地区毫不松懈地抓好防汛抗洪和灾后生产恢复，疏通水渠、清理杂物、抢收早稻、补种晚稻……　　“洪水一退我们就下田了，我有信心晚稻一定能丰收。”信心来自哪里？中央财政下达农业生产和水利救灾资金8.3亿元，支持灾区恢复生产；农业部门做好救灾种子调剂调运，保障大田用种；地方党委政府派出党员干部突击队、组织农机农资农技人员，全力帮扶受灾群众；机械作业、秧盘种植，农业科技为抢抓农时提供保障。更重要的是，只要抢抓时机、肯出力气，就一定能换来收获。　　直面洪灾，挺起的是脊梁；决胜小康，不变的是信念。用一颗</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">			
+http://opinion.people.com.cn/n1/2020/0810/c1003-31815910.html</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>“大家富才是真的富”</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？周珊珊　　【人物】致富带头人塔依尔・卡吾里　　【故事】塔依尔・卡吾里，是新疆维吾尔自治区克孜勒苏柯尔克孜自治州阿克陶县塔尔塔吉克民族乡库祖村村民。几年前，他被村里列为建档立卡的贫困户，后来外出务工，积累了一些收入，生活也越来越好。他认为，自己富起来不算富，大家富才是真的富。于是在2014年，他带领12名贫困群众外出务工3个月，人均收入达到1.6万元；2015年带领15名贫困群众务工2个月，人均收入达到1.5万元。此后，他带领当地村民务工增收、鼓励村民参加技术培训、为村里平整道路、帮村里建起学校等，为村民铺就了致富路。2019年，塔依尔・卡吾里荣获全国脱</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/n1/2020/0810/c1003-31815911.html</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>始终心中装有群众</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">登录人民网通行证    立即注册忘记密码？张军斌　　今年3月，习近平总书记在浙江考察时来到安吉县社会矛盾纠纷调处化解中心，了解群众矛盾纠纷一站式接收、一揽子调处、全链条解决模式运行情况。习近平总书记强调，让老百姓遇到问题能有地方“找个说法”，切实把矛盾解决在萌芽状态、化解在基层。　　司法是维护社会公平正义的最后一道防线。人民法院是给老百姓“说法”的地方，应该守好这一防线。可以说，给出一个让老百姓满意的“说法”，既是人民法院坚持以人民为中心的发展思想的必然要求，也是保障国家长治久安、社会安定有序、人民安居乐业的重要途径。站稳群众立场，人民法院要回答好“给什么”“怎么给”“给得怎么样”的问题。　　</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/n1/2020/0810/c1003-31815944.html</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>耕耘好梦想的“菜地”</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？李远哲　　图为张亚东正在组装自己预先制好的高架桥模型部件。该桥梁模型规划总长度18米，建成后将铺设高铁轨道模型。　　本报记者  毕京津摄　　梦想对每个人都敞开怀抱，但要实现梦想却没那么轻松，需要勇敢守护、长期坚持　　　　近日，一则视频引发关注。主人公张亚东是郑州电力职业技术学院的大一学生，由于酷爱机电模型，疫情防控期间，他在屋后一片菜地里动手施工，建出一系列微缩版基建工程。不仅有铁路、隧道，甚至还有跨江大桥。风行网络之后，大家称之为“菜地里的奇观”，很多人钦佩他：好厉害！　　张亚东在这片菜地里耕耘的，正是他的爱好、他的梦。　　心里有梦，便有强烈的兴趣推</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/GB/223228/index.html</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>网评</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿¿ªÀ¸Óï£º´ó¼ÒºÃ£¬ÎÒÊÇÐ¡½¯¡£¹úÊÂ£¬¼ÒÊÂ£¬ÌìÏÂÊÂ£¬ÌìÌì¶¼ÓÐÐÂÏÊÊÂ¡£ÄãÆÀ£¬ÎÒÆÀ£¬ÖÚÈËÆÀ£¬°Ù»¨Æë·ÅÈÎ¾ýÆ·¡£</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t xml:space="preserve">		
+http://opinion.people.com.cn/n1/2020/0810/c1003-31815906.html</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>人不负青山 青山定不负人</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？本报评论部　　2005年8月15日，时任浙江省委书记习近平在安吉余村考察时强调：“我们过去讲既要绿水青山，又要金山银山，实际上绿水青山就是金山银山。”今年8月15日，是“两山论”提出15周年，“两山论”丰富发展成为习近平生态文明思想，中国的生态文明建设也取得了举世瞩目的成就。即日起，本版推出系列评论，共话生态文明、共建美丽中国。　　――编  者  　　  　　习近平生态文明思想回答了中国发展最重要的时代之问，也契合了经济转型升级的规律、顺应了人们对美好生活的期待            　　一个村庄的变化，可以折射一个国家的变迁。上世纪70年代开始，浙江</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/GB/427456/index.html</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>财评</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿¿ªÀ¸Óï£º´ó¼ÒºÃ£¬ÎÒÊÇÐ¡½¯¡£¹úÊÂ£¬¼ÒÊÂ£¬ÌìÏÂÊÂ£¬ÌìÌì¶¼ÓÐÐÂÏÊÊÂ¡£ÄãÆÀ£¬ÎÒÆÀ£¬ÖÚÈËÆÀ£¬°Ù»¨Æë·ÅÈÎ¾ýÆ·¡£</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/n1/2020/0809/c427456-31815626.html</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>办好自己的事是战胜风险挑战的根本</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？叶敖	越是面对压力，越要保持定力；越是乱云飞渡，越要集中力量办好自己的事。	7月30日，中共中央政治局召开会议，分析研究当前经济形势，部署下半年经济工作。向内看，我国经济正处在转变发展方式、优化经济结构、转换增长动力的攻关期，面临着结构性、体制性、周期性问题相互交织所带来的困难和挑战；向外看，我们还要面对世界经济深度衰退、国际贸易和投资大幅萎缩、国际金融市场动荡、国际交往受限、经济全球化遭遇逆流、一些国家保护主义和单边主义盛行、地缘政治风险上升等不利局面。在一个更加不稳定不确定的世界中谋求发展，战胜各种风险挑战，最根本的还是办好我们自己的事情。	办好自</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/GB/159301/index.html</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>快评</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿¿ªÀ¸Óï£º´ó¼ÒºÃ£¬ÎÒÊÇÐ¡½¯¡£¹úÊÂ£¬¼ÒÊÂ£¬ÌìÏÂÊÂ£¬ÌìÌì¶¼ÓÐÐÂÏÊÊÂ¡£ÄãÆÀ£¬ÎÒÆÀ£¬ÖÚÈËÆÀ£¬°Ù»¨Æë·ÅÈÎ¾ýÆ·¡£</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/GB/1036/index.html</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>热议</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿¿ªÀ¸Óï£º´ó¼ÒºÃ£¬ÎÒÊÇÐ¡½¯¡£¹úÊÂ£¬¼ÒÊÂ£¬ÌìÏÂÊÂ£¬ÌìÌì¶¼ÓÐÐÂÏÊÊÂ¡£ÄãÆÀ£¬ÎÒÆÀ£¬ÖÚÈËÆÀ£¬°Ù»¨Æë·ÅÈÎ¾ýÆ·¡£</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	
+http://opinion.people.com.cn/n1/2020/0810/c1003-31815908.html</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>用高质量发展吸引高素质人才</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？富子梅　　前不久，天津公布上半年经济社会发展数据，总体呈现质量向好、结构向优的发展态势。统筹推进疫情防控和经济社会发展，天津取得产业结构持续优化、新动能成长势头良好的成绩，提振了干部群众实现高质量发展的信心。　　近年来，天津在结构调整、产业转型上“咬定青山不放松”，对新发展理念的认识日益深化，对创新驱动规律的把握与时俱进。注重发展质量和发展效益，坚定走高质量发展之路，做足智能化、大数据、云计算的文章，用新技术赋能传统产业，在原有制造业门类齐全的基础上，智能制造异军突起，创新发展的生态链正逐步形成并日臻完善。　　招商引资重“智”。城市发展，人才是千秋大计</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/GB/431649/index.html</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>来论</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿¿ªÀ¸Óï£º´ó¼ÒºÃ£¬ÎÒÊÇÐ¡½¯¡£¹úÊÂ£¬¼ÒÊÂ£¬ÌìÏÂÊÂ£¬ÌìÌì¶¼ÓÐÐÂÏÊÊÂ¡£ÄãÆÀ£¬ÎÒÆÀ£¬ÖÚÈËÆÀ£¬°Ù»¨Æë·ÅÈÎ¾ýÆ·¡£</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	
+http://opinion.people.com.cn/n1/2020/0810/c1003-31815969.html</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>牢牢稳住粮食安全压舱石</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？■ 李 婕　　“我十分关心粮食生产和安全。今年夏粮丰收大局已定，秋粮要争取有好的收成。”近日，习近平总书记在吉林考察，第一站就来到松辽平原，了解粮食生产，体现了对粮食安全的高度重视。　　十几亿人口要吃饭，这是中国最大的国情。“手中有粮、心中不慌”在任何时候都是真理，今年更有着特殊的意义。在疫情防控的特殊时期，即便春节后叠加物流、零售等行业人手紧张，中国的粮食价格依然保持总体平稳，市场运行快速恢复。“米面随买随有”“粮食还是吃新的好”，关键时刻的良好表现让大家宽了心。这背后最大的支撑力，源自中国粮食产量丰、库存足，源自我们牢牢守护的粮食安全。　　外部环境</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>http://opinion.people.com.cn/GB/8213/119388/index.html</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>1+1</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    开栏的话：大家好，我是小蒋。国事，家事，天下事，天天都有新鲜事。你评，我评，众人评，百花齐放任君看。观点各有不同，角度各有侧重，只要我们尊重客观、理性公正。  
+　人民日报社概况|关于人民网|报社招聘|招聘英才|广告服务|合作加盟|供稿服务|网站声明|网站律师|呼叫中心|ENGLISH镜像:日本  教育网  科技网  服务邮箱  kf@people.cn  违法和不良信息举报电话：010-65363263互联网新闻信息服务许可证1012006001|增值电信业务经营许可证B2-20100025信息网络传播视听节目许可证0104065|广播电视节目制作经营许可证（广媒）字第172号网络文</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t xml:space="preserve">http://opinion.people.com.cn/n1/2020/0810/c1003-31817179.html
+</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>教师做微商，要“堵”也要“疏”</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？蒋萌	       浙江乐清一老师在上班时间开展微商兼职经营活动，部分学生家长由其介绍加入微信购物群或实际购买产品，被学生家长投诉至当地教育局纪检监察组，有关教师被立案查处。	       “瓜田不纳履，李下不整冠。”老师（尤其是公立学校的老师）的本职工作是教书育人。如果老师兼做微商，学生和家长很可能会成为潜在“客户”，事情很可能“串味儿”――容易影响正常教学，学生“三观”也容易受到不良影响，值得警惕。	       2018年11月8日，教育部印发《新时代中小学教师职业行为十项准则》明确规定，教师不得擅自从事影响教育教学本职工作的兼职兼薪行为，不得利</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	 http://politics.people.com.cn/n1/2020/0810/c1001-31815883.html</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	 http://politics.people.com.cn/n1/2020/0810/c1001-31815883.html</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>HTTP ERROR</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815882.html</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815882.html</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
+          <t>HTTP ERROR</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815884.html</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815884.html</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
+          <t>HTTP ERROR</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815886.html</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815886.html</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
+          <t>HTTP ERROR</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815888.html</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>http://politics.people.com.cn/n1/2020/0810/c1001-31815888.html</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
+          <t>HTTP ERROR</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>http://travel.people.com.cn/n1/2020/0810/c41570-31817016.html</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>15部门:稳农民工就业 推动乡村游健康发展</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿	ÈËÃñÍø±±¾©8ÔÂ10ÈÕµç £¨¼ÇÕßÁõ¼Ñ£©¼ÇÕß´ÓÎÄ»¯ºÍÂÃÓÎ²¿»ñÏ¤£¬ÈËÁ¦×ÊÔ´ºÍÉç»á±£ÕÏ²¿¡¢¹ú¼Ò·¢Õ¹ºÍ¸Ä¸ïÎ¯Ô±»á¡¢ÎÄ»¯ºÍÂÃÓÎ²¿µÈ15²¿ÃÅÈÕÇ°ÁªºÏÓ¡·¢µÄ¡¶¹ØÓÚ×öºÃµ±Ç°Å©Ãñ¹¤¾ÍÒµ´´Òµ¹¤×÷µÄÒâ¼û¡·£¨ÒÔÏÂ¼ò³Æ¡¶Òâ¼û¡·£©Ìá³ö£¬¼Ó´ó¶Ô×¡ËÞ²ÍÒû¡¢ÎÄ»¯ÂÃÓÎµÈÐÐÒµµÄÕë¶ÔÐÔÕþ²ß·ö³Ö£¬×î´óÏÞ¶ÈÎÈ¶¨Å</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>http://legal.people.com.cn/n1/2020/0810/c42510-31817071.html</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>两部门启动长江非法捕捞同步巡查执法行动</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 （薄晨棣）记者从公安部获悉，8月10日上午，由公安部、农业农村部打击长江流域非法捕捞专项整治行动工作专班部署开展的长江流域非法捕捞高发水域同步巡查执法行动正式启动。	按照统一部署，首轮巡查执法行动为期15天，由长江流域非法捕捞高发水域相关省市公安机关、渔业主管部门以及上下游、左右岸、干支流的水上执法力量同步组织开展。公安机关等部门执法船艇将加大对重点水域的执法频度，扩大执法覆盖面，有效遏制非法捕捞多发高发态势，切实维护长江流域禁捕秩序。仅8月10日上午，就出动公安、渔政等执法力量6100余人次，执法船艇497艘次，现场查处非法</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>http://auto.people.com.cn/n1/2020/0810/c1005-31816845.html</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>8部门:制定快递包装材料无害化标准体系</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电（王紫）近日，市场监管总局、发展改革委、科技部、工业和信息化部、生态环境部、住房城乡建设部、商务部、国家邮政局等八部门联合印发《关于加强快递绿色包装标准化工作的指导意见》（以下简称《意见》），提出到2022年年底前，制定实施快递包装材料无害化强制性国家标准，基本建立覆盖全面、重点突出、结构合理的快递绿色包装标准体系。	据估算，我国快递业每年消耗的纸类废弃物超过900万吨、塑料废弃物约180万吨，并呈快速增长趋势，对环境造成的影响不容忽视。加强快递绿色包装标准化工作，支撑妥善处理快递包装污染问题，已成为行业转型升级、可持续发展的内</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>http://culture.people.com.cn/n1/2020/0810/c1013-31815933.html</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>国家电影局、中国科协:促进科幻电影发展</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？　　本报北京8月9日电  （记者刘阳）近日，国家电影局、中国科协印发《关于促进科幻电影发展的若干意见》（以下简称《意见》），提出将科幻电影打造成为电影高质量发展的重要增长点和新动能，把创作优秀电影作为中心环节，推动我国由电影大国向电影强国迈进。《意见》具体提出10条加强扶持引导的政策措施，被称为“科幻十条”。　　在创作生产方面，《意见》要求加大对科幻电影剧本的培育力度，鼓励扶持原创，促进科幻文学、动漫、游戏等资源转化，丰富科幻电影的内容创新源头，推动建立多层次多样化可持续的科幻电影剧本供给体系。支持在夏衍杯优秀电影剧本征集、扶持青年优秀电影剧作计划、电</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>http://legal.people.com.cn/n1/2020/0810/c42510-31815931.html</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>"昆仑2020"行动抓获犯罪嫌疑人4.3万余名</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？　　本报北京8月9日电  （记者张璁）今年5月，公安部部署全国公安机关开展“昆仑2020”专项行动，依法严厉打击危害食品、药品、生态环境安全，侵犯知识产权和涉野生动植物等领域违法犯罪。全国公安机关全环节全要素全链条打击，破获一批大要案件。截至目前，共破获刑事案件2.4万余起，捣毁违法犯罪窝点7400余个，打掉犯罪团伙3000余个，抓获犯罪嫌疑人4.3万余名，涉案总价值185亿元。　　在打击危害食品安全犯罪活动领域，公安机关重点针对肉制品、食用油、保健食品、酒水饮料等领域的犯罪行为，主动作为、重拳出击，共破获案件4700余起，捣毁窝点2600余个，打掉犯</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31815914.html</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>读者来信:"断头路"问题亟待进一步重视</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？沈童睿	　　近来，本报收到不少读者来信，反映“断头路”问题：有的是生活小区通往城市主干道的道路修到一半停工了，原本不过几十米的路程，如今却要绕道走十几分钟；有的是农村地区道路硬化不到位，一到下雨天，道路就泥泞不堪，影响出行，等等。	　　交通是发展问题，也是民生问题。近年来，各地各部门在完善城市农村路网交通方面做了大量工作，无论是百姓出行，还是城乡经济社会发展，都大为便利。不过，从读者来信的反映看，一些地方的交通“微循环”还有待改善，“断头路”问题亟待进一步重视并积极加以解决。	　　造成“断头路”的原因有很多。有的是养护工作不到位，道路年久失修，破损严重</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31817254.html</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>暴雨蓝色预警:闽川大暴雨</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 中央气象台8月10日18时发布暴雨蓝色预警：	预计，8月10日20时至11日20时，青藏高原东部、甘肃南部、四川盆地西部、内蒙古西部、福建中南部、台湾岛大部以及江淮南部、江南北部、广西北部、黑龙江中部、云南西部等地的部分地区有大到暴雨，其中，福建东南部、四川盆地西部、甘肃南部等地局地有大暴雨（100～180毫米）。上述部分地区伴有短时强降水（最大小时降雨量30～50毫米，局地可超过70毫米），局地有雷暴大风等强对流天气。防御指南：	1、建议政府及相关部门按照职责做好防御暴雨应急工作；	2、切断有危险地带的室外电源，暂停户外作业</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31817256.html</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>台风黄色预警</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 中央气象台8月10日18时发布台风黄色预警：	南海热带低压已于今天（10日）上午加强为今年第6号台风“米克拉”（英文名称：Mekkhala；名字来源：泰国；名字意义：雷天使），下午5点钟“米克拉”由热带风暴级加强为强热带风暴级，其中心位于福建厦门偏南方约390公里的海面上，就是北纬21.0度、东经118.5度，中心附近最大风力有10级（25米/秒），中心最低气压为985百帕，七级风圈半径200-270公里。	预计，“米克拉”将以每小时25-30公里的速度向偏北方向移动，强度还将有所加强，将于11日早晨到上午在福建漳浦到平潭一带</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>http://it.people.com.cn/n1/2020/0810/c1009-31816802.html</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>网信办查处在线学习违法违规平台</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 （记者杨虞波罗）记者从国家网信办官网获悉，有部分学习教育类网站平台和APP主体责任意识淡漠，在利益驱使下，借机传播一些有害和不良信息，恶意弹窗引流，严重干扰青少年正常学习，为广大群众深恶痛绝。针对上述问题，国家网信办在7月初启动的2020“清朗”未成年人暑期网络环境专项整治中，聚焦网站平台网课学习频道、学习教育类APP、工具类应用弹窗等未成年人常用的环节和应用，在前期处置“学而思网校”APP基础上，近日依法查处了一批影响恶劣的网站平台。有关典型案例公布如下：7家网站平台网课学习频道推送导向不良信息，故意利用色情低俗、暴力恐怖等</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31815892.html</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>43家外资金融机构确认参加服贸会专题展</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？　　本报北京8月9日电  （记者王昊男）截至目前，2020中国国际服务贸易交易会已有100余家国际国内金融机构参加线上线下展览展示。其中，来自18个国家和地区的43家外资金融机构参展，金融服务展综合展区国际化率超60%。　　据介绍，创办于2005年的北京国际金融论坛今年纳入服贸会，将作为2020年服贸会金融服务专题展举办。金融服务专题展作为2020年服贸会8个专题展之一，以“新金融、新开放、新发展”为主题，展会三路并进，包括组织展览展示、论坛交流等。金融板块展览总面积6555平方米，综合展区555平方米，户外展区有6000平方米。　　在展示主题上，将集</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>http://bj.people.com.cn/n2/2020/0810/c14540-34217134.html</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>北京拟严管短租房 开民宿或需业主同意</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电（池梦蕊）最近几年，短租民宿平台兴起，一些住宅小区的住房也被改成短租民宿经营。同时一些中介也推出了“短租公寓”的产品。此前，对于短租民宿，缺少相关的规范管理。而如今，短租民宿、公寓将迎来最严的监管。	今天，北京市住建委、北京市公安局、北京市网信办今日联合公布《关于规范管理短租住房的通知》（征求意见稿），向社会公开征求意见。	其中规定，经营短租房要符合小区管理规约或业主大会决定，没有管理规约或业主大会决定的，要取得同楼其他业主书面同意。	根据征求意见稿，短租住房是指利用国有土地上的居住小区内的住房，按日或者小时收费，提供住宿休息服</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31815872.html</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>西安明秦王府城墙坍塌:近期连续大雨所致</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？李华、吴鸿波、杨一苗	　　新华社西安8月8日电 记者8日晚从西安市文物局了解到，8日上午发生坍塌的明秦王府城墙经专家现场勘察，认定坍塌原因为近期连续大雨所致，坍塌部分为原城墙遗址新筑保护性土体和东北侧外包砖砌体，未伤及原明代城墙夯土。	　　8月8日，工作人员在西安市新城广场明秦王府城墙遗迹坍塌事故现场清理路面。新华社记者 李一博 摄	　　此段坍塌区域为陕西省文物保护单位明秦王府城墙遗址南墙西段修复保护砌体，位于西安市新城广场西南侧，并非全国重点文物保护单位西安城墙。坍塌前，相关部门已按规范在现场设立警戒线，准备雨后进场加固。经专家现场勘察，判定明秦王府</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0810/c1008-31816066.html</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>内蒙古希拉穆仁镇遭龙卷风袭击 33人受伤</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电  据达茂联合旗委员会宣传部官方微信消息，8月9日下午15点30分左右，达茂旗希拉穆仁镇呼和点素嘎查遭受龙卷风袭击。据初步统计，灾害造成呼和点素嘎查5户牧民受灾，天鹅湖旅游接待点受灾较为严重。天鹅湖旅游接待点游客、景点服务员、工作人员33人不同程度受伤，100余顶蒙古包倾倒或受损。	灾害发生后，自治区人大常委会副主任、市委书记张院忠立即作出指示，要求达茂旗委、旗政府立即组织开展灾害救援和善后工作，快速转移和救治受灾群众，并派出市领导赶赴现场。达茂旗委、旗政府紧急成立了现场搜救组、医疗救治组、善后处置组等工作组，旗委、政府主要领导</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>http://rmfp.people.com.cn/n1/2020/0810/c406725-31817111.html</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>全国扶贫职业技能大赛:技能促就业助脱贫</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	发布会现场	人民网北京8月10日电 （记者 史雅乔）10日下午，由人力资源和社会保障部、国务院扶贫开发领导小组办公室联合主办，山西省人力资源和社会保障厅、山西省扶贫开发办公室、大同市人民政府承办的全国扶贫职业技能大赛（以下简称“大赛”）举行媒体见面会，通报大赛相关情况并回答有关问题。人社部职业能力建设司司长、大赛组委会副主任张立新，山西省人社厅厅长、大赛组委会副主任、大赛执委会常务副主任卢建明，国务院扶贫工作领导小组办公室开发指导司副司长、大赛组委会委员刘晓山，山西省大同市政府常务副市长、大赛执委会副主任薛明耀出席见面会。	记者获悉，本次大赛将于8月</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>http://money.people.com.cn/n1/2020/0810/c42877-31816935.html</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>服贸会专题展吸引百余家金融机构参加</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	图为2020中国国际服务贸易交易会金融服务专题展首场媒体通气会。（人民网记者 李彤摄）	人民网北京8月10日电 （记者李彤）近日，2020中国国际服务贸易交易会金融服务专题展首场媒体通气会在京举行。记者从会上了解到，将于9月上旬在北京国家会议中心举办的专题展，有18个国家和地区的100余家金融机构参加线上线下展览。展会设置国家金融管理中心展区、金融业支持全球服务贸易展区、未来金融与智慧金融展区、全球财富管理展区、金融业对外开放展区五大展区。	据了解，由商务部和北京市人民政府共同主办的中国国际服务贸易交易会是全球首个服务贸易领域的综合性展会，是中国服务</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+http://health.people.com.cn/n1/2020/0810/c14739-31815877.html</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>心脏累了吗?警惕!这些症状说明心脏有事</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
+          <t>编者按：心脏病的危害早已为人所熟知，但对其表现出的症状，很少有人能弄明白，以至于有的人已出现心脏病症状，却浑然不知，什么症状才是心脏病，如何正确判断？什么症状说明心脏不好1.有胸闷、心慌、胸痛的症状，就是心脏病吗？	不一定。北京中医药大学心血管病研究所所长王显表示，心脏病的常见症状包括胸闷、心慌、胸痛，但出现这些症状，不代表就是心脏病，也可能是神经功能调节失衡所引起。另外，剧烈运动、过度劳累时也会出现胸闷、心慌，但需要区别的是，非心脏器质性病变引起的胸闷、心慌持续时间不会很长，休息后可能就会好转，而心脏病患者活动量大时会加重不适。因此建议，为了保险起见，出现该症状的人应该去医院进一步诊断，以明</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/n1/2020/0810/c40531-31816717.html</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>理论聚焦：党的伟大历史实践与时代探索</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合林雅华（中央党校文史部 副教授）2020年08月10日09:30    来源：中国青年报	新时代中国共产党的历史使命，不仅是传统中国的担道情怀与天下关怀的现代书写，同时也是一个来自人民的现代政党向未来中国与人类文明，所交出的一份时代答卷。	---------------	十月革命之后，马克思主义来到中国。面对中华民族日益深重的忧患，中国共产党以马克思主义理论为指导，带领中国人民走上了争取民族自由解放、重建民族文化主体性地位、推进中华文明</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
+          <t>http://dangjian.people.com.cn/GB/136058/431693/index.html</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>创建模范机关：</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
+          <t>Ö÷°ìµ¥Î»£ºÖÐÑëºÍ¹ú¼Ò»ú¹Ø¹¤Î¯Ðû´«²¿³Ð°ìµ¥Î»£ºÈËÃñÍø¡¢ÐÂ»ªÍø¡¢¹²²úµ³Ô±Íø¡¢µ³½¨Íø¡¢ÆìÖÄÍø    ÖÐÑëºÍ¹ú¼Ò»ú¹Ø¸÷¼¶µ³×éÖ¯ºÍ¹ã´óµ³Ô±¸É²¿ÈÏÕæ¹á³¹ÂäÊµÏ°½üÆ½×ÜÊé¼ÇÖØÒªÖ¸Ê¾¾«Éñ£¬ÒÔ¸ß¶ÈµÄÕþÖÎÔðÈÎ¸Ð¡¢Ê¹Ãü¸Ð£¬°ÑÒßÇé·À¿Ø×÷Îªµ±Ç°×îÖØÒªµÄ¹¤×÷À´×¥¡­¡­    ÖÐÑëºÍ¹ú¼Ò»ú¹Ø¹á³¹ÂäÊµÏ°½üÆ½×ÜÊé¼ÇÖØÒªÖ¸Ê¾¾«Éñ¼á¾ö´òÓ®ÒßÇé·À¿Ø×è</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
+          <t>http://dangjian.people.com.cn/n1/2020/0810/c117092-31816205.html</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>务实高效推进科技交流合作</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:09    来源：旗帜网	　　习近平总书记在中央和国家机关党的建设工作会上强调“要围绕中心抓党建、抓好党建促业务，坚持党建工作和业务工作一起谋划、一起部署、一起落实、一起检查。”“欲筑室者，先治其基”，推进党建与业务融合，关键是找准结合点，将基层党组织对党员的教育、管理、监督等基本职责渗透到业务工作中去，将组织、宣传、凝聚、服务群众的职责贯穿于业务工作的全过程。通过基层党组织的标准化规范化建设，可以有效引领业</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B86" t="inlineStr">
+        <is>
+          <t>http://renshi.people.com.cn/n1/2020/0810/c139617-31816305.html</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>黑龙江省委组织部发布一批干部任前公示</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:21    来源：黑龙江日报	依据《党政领导干部选拔任用工作条例》规定，为加强干部选拔任用工作的民主监督，现将拟任职的干部进行任前公示（按姓氏笔画为序），公示期限为2020年8月10日―2020年8月14日（5个工作日）。	马存新 男，汉族，1966年7月生，54岁，1989年7月参加工作，1989年1月入党，省委党校经济管理专业研究生毕业，现任省纪委监委办公厅主任（副厅长级），拟转任省直机关副厅级领导职务。</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B87" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/GB/40557/431524/433440/index.html</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>理论圆桌会：打赢脱贫攻坚战要精准施策</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
+          <t xml:space="preserve">       集理论之思，汇大家之言。本期《理论圆桌会》聚焦打赢脱贫攻坚战的精准施策，敬请关注。       脱贫攻坚贵在精准重在精准，成败之举在于精准。用好精准之方，应以非常之力、关键之举继续在精准施策上出实招、在精准推进上下实功、在精准落地上见实效。      中国社会科学院经济研究所副所长胡乐明认为：脱贫攻坚难在精准、贵在精准、重在精准。如期完成脱贫攻坚历史性任务，要求各地必须结合自身发展的实际情况，坚持精准施策，狠抓落实，有效提升脱贫质量，以非常之力、关键之举实现全面胜利。应该看到，剩余贫困地区和贫困人口大都具有“成因复杂多变、贫困程度深、蔓延久、分布广、类型各异”的特征，全面如期完成</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/n1/2020/0810/c40531-31816246.html</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>在学思践悟中坚定共产党人的理想信念</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合秦彪生2020年08月10日08:12    来源：人民网-理论频道	今年“七一”前夕，习近平总书记在给复旦大学《共产党宣言》展示馆党员志愿服务队全体队员的回信中指出，希望广大党员特别是青年党员认真学习马克思主义理论，结合学习党史、新中国史、改革开放史、社会主义发展史，在学思践悟中坚定理想信念，在奋发有为中践行初心使命，努力为实现“两个一百年”奋斗目标、实现中华民族伟大复兴的中国梦贡献智慧和力量。	历史是最好的教科书，树立坚定的理想信念</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>http://fanfu.people.com.cn/n1/2020/0810/c64371-31816826.html</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>观察:今年以来,资源领域多名官员接连落马</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日10:02    来源：中央纪委国家监委网站8月6日，云南省自然资源厅土地储备中心副主任周敏接受监察调查；7月28日，四川省煤炭产业集团有限责任公司党委书记、董事长景宏年接受纪律审查和监察调查；7月14日，山西省大同煤矿集团党委委员张良海接受审查调查……今年以来，煤炭、石油、矿产等领域多名官员接连落马，资源领域反腐败成绩单引发关注。	资源领域资金密集、权力集中、审批环节多，容易成为违纪违法行为的高发地。十九届中央纪</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>http://fanfu.people.com.cn/n1/2020/0810/c64371-31816189.html</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>青海木里矿区非法开采多名涉事干部被免职</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:06    来源：中央纪委国家监委网站8月9日下午，记者获悉，针对媒体报道木里矿区非法开采问题，青海省纪委监委已成立调查组，对涉嫌失职失责等问题立案调查。目前，多名涉事干部被免职。涉事企业涉嫌非法开采，破坏生态环境，公安机关依法已经对马少伟等相关责任人采取强制措施。	此前，有媒体报道称，一家名为青海省兴青工贸工程集团有限公司的企业，打着生态修复治理的名义，在祁连山南麓腹地木里矿区进行掠夺式采挖，获利上百亿元人</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/n1/2020/0810/c40531-31816210.html</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>建设美丽中国:人不负青山 青山定不负人</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合本报评论部2020年08月10日08:09    来源：人民网－人民日报	2005年8月15日，时任浙江省委书记习近平在安吉余村考察时强调：“我们过去讲既要绿水青山，又要金山银山，实际上绿水青山就是金山银山。”今年8月15日，是“两山论”提出15周年，“两山论”丰富发展成为习近平生态文明思想，中国的生态文明建设也取得了举世瞩目的成就。即日起，本版推出系列评论，共话生态文明、共建美丽中国。	――编  者  	习近平生态文明思想回答了中国发</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B92" t="inlineStr">
+        <is>
+          <t>http://renshi.people.com.cn/n1/2020/0810/c139617-31816352.html</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>广东省发布省政府7月干部职务任免</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:27    来源：人民网-中国共产党新闻网	中国共产党新闻网北京8月10日电　(任佳晖)近日，广东省人力资源和社会保障厅网站发布广东省政府7月人事任免，具体情况如下：省政府2020年7月份任命：	黄海 广东省公安厅刑事侦查局局长，试用1年	沙伟春 广东省公安厅治安管理局局长，试用1年	杨海 广东省体育局副局长	张名位 广东省农业科学院副院长	黎孟枫 南方医科大学校长	阮双琛 深圳技术大学校长	杨洲 嘉应学院院</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B93" t="inlineStr">
+        <is>
+          <t>http://renshi.people.com.cn/n1/2020/0810/c139617-31816238.html</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>张勇、刘国周任广东省深圳市副市长(简历)</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
+          <t xml:space="preserve">高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:12    来源：人民网-中国共产党新闻网	中国共产党新闻网北京8月10日电　(任佳晖)据《深圳特区报》消息，近日，深圳市第六届人民代表大会常务委员会第四十三次会议表决通过，决定任命：张勇为深圳市人民政府副市长；刘国周为深圳市人民政府副市长、市公安局局长。张勇同志简历	张勇，男，汉族，1974年5月生，山西临县人，1995年5月入党，1995年7月参加工作，湖南大学交通土建工程专业毕业，大学学历，工程硕士。	</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B94" t="inlineStr">
+        <is>
+          <t>http://fanfu.people.com.cn/n1/2020/0810/c64371-31816347.html</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>湖南省四名干部涉严重违纪违法被查</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:25    来源：人民网-中国共产党新闻网	中国共产党新闻网北京8月10日电   (扶婧颖)近日，湖南省纪委监委网站发布四名干部涉嫌严重违纪违法接受审查调查的消息，具体内容如下：湖南省桃源县市场监督管理局公平交易执法中队队长吴智斌主动投案	湖南省桃源县市场监督管理局公平交易执法中队队长吴智斌涉嫌严重违纪违法，主动投案，目前正配合桃源县纪委监委纪律审查和监察调查。湖南省桃源县委政法委原副书记游建国主动投案	湖南</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B95" t="inlineStr">
+        <is>
+          <t>http://fanfu.people.com.cn/n1/2020/0810/c64371-31816232.html</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>雁过拔毛 国企原董事长敛财千万获刑19年</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合2020年08月10日08:11    来源：中央纪委国家监委网站	8月1日，四川省原新津县（现新津区）国有资产投资经营有限责任公司董事长、总经理，成都新诚融资担保有限公司原董事长、总经理王利志，本应当和战友相聚共忆峥嵘岁月，然而与以往过节的热闹欢乐不同，今年王利志独自在看守所，只有铁窗和悔恨相伴。	一年多前，他收到开除党籍、开除公职的处分决定。	本该站好“最后一班岗”的国企领导干部，为何被一纸处分决定画上了42年工作的句点？一个曾宣誓</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/n1/2020/0810/c40531-31816202.html</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>构建乡村和小城镇联动发展的机制</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合黄凯南2020年08月10日08:08    来源：光明日报【光明论坛】	乡村振兴战略和新型城镇化战略双轮驱动构成了新时代我国经济高质量发展的重要引擎，两大战略的协同推进是解决我国区域和城乡发展不平衡不充分、实现城乡融合发展的重要战略部署。在新的发展时期，小城镇发展的意义和作用更为特殊，发挥着上接县城、下连村庄的纽带作用，既是新型城镇化的末梢，又是乡村振兴就地城镇化的直接载体。	小城镇与其所管辖的村庄无论是物理空间还是经济、社会、文化和</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr">
+        <is>
+          <t>http://theory.people.com.cn/n1/2020/0810/c40531-31816187.html</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>弘扬优良家风 营造见贤思齐的社会氛围</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合刘琳2020年08月10日08:06    来源：光明日报	《新时代公民道德建设纲要》（以下简称《纲要》）提出要用良好家教家风涵育道德品行，这是新时代公民道德建设实践中深化道德教育引导的重要方面。习近平总书记高度重视家风建设，他以中华优秀传统家风文化为营养源泉，立足马克思主义家庭观和中国共产党人的红色家风，围绕家风建设作出了一系列重要论述，为新时代公民道德建设提供了根本遵循。一	党的十八大以来，习近平总书记多次强调家风建设的重要性，20</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B98" t="inlineStr">
+        <is>
+          <t>http://dangshi.people.com.cn/n1/2020/0810/c85037-31816119.html</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>八路军桂林办事处：生动再现历史</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合本报记者  庞革平2020年08月10日07:50    来源：人民网－人民日报	广西桂林市区中山北路14号，坐落着一幢白色两层砖木楼房，桂北民居建筑风格，气质笃厚、安静。这里曾是一个卖酒铺子，伫立于此已有八十余载，它见证了国共两党第二次合作，见证了桂林人民如火如荼的抗日救亡运动。这座楼房还有一个更为令人瞩目的身份――八路军桂林办事处旧址。	1938年10月，随着广州、武汉等城市的相继沦陷，抗战已转入相持阶段。1938年11月，在周恩来</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B99" t="inlineStr">
+        <is>
+          <t>http://dangshi.people.com.cn/n1/2020/0810/c85037-31816148.html</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>钱壮飞:打入敌人"心脏" 龙潭虎穴挽狂澜</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
+          <t>高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合高层动态干部论坛人事理论党建群团独家视频部委信息领导活动反腐评论党史先锋滚动综合潘宏2020年08月10日07:59    来源：学习时报	　　钱壮飞是中国共产党早期隐蔽战线斗争的杰出代表，他的机智勇敢令人感佩，他的英雄业绩令人肃然起敬。周恩来曾把他与李克农、胡底并列为党的情报工作“龙潭三杰”。凭着对革命事业的赤胆忠心，钱壮飞深入龙潭虎穴，为保卫党中央的安全作出了卓越贡献，他的功绩永远铭刻于中国革命史册。	　　革命路上的同道伉俪	　　钱壮飞1896年出生于浙江湖州商人家庭，本名钱壮秋，又名钱潮。他机智幽默而擅应酬，</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B100" t="inlineStr">
+        <is>
+          <t>http://dangjian.people.com.cn/GB/136058/429005/index.html</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>第五届全国基层党建创新案例</t>
+        </is>
+      </c>
+      <c r="D100" t="inlineStr">
+        <is>
+          <t>¾­¹ýÍøÉÏÕ¹Ê¾¡¢ÍøÉÏ¹«Ê¾¡¢³õÆÀ¡¢¸´ÆÀºÍÖÕÆÀµÈ»·½Ú£¬×îºóÆÀ³öÈ«¹ú»ù²ãµ³½¨´´ÐÂ×î¼Ñ°¸ÀýºÍÓÅÐã°¸Àý¹²80¸ö£¬ÆäÖÐ×î¼Ñ°¸Àý30¸ö¡¢ÓÅÐã°¸Àý50¸ö¡£ÏÖ½«ÆÀÑ¡½á¹ûÓèÒÔ¹«²¼¡£¡°ÌáÉý»ù²ãµ³×éÖ¯×éÖ¯Á¦¡±ÑÐÌÖ»áôßµÚÎå½ìÈ«¹ú»ù²ãµ³½¨´´ÐÂµäÐÍ°¸ÀýÕ÷¼¯ÆÀÑ¡»î¶¯Æô¶¯ÒÇÊ½9ÔÂ19ÈÕÔÚ¹ãÎ÷¹ó¸Û³É¹¦¾ÙÐÐ¡£¡¡¡¡ºþÄÏÓÀË³ÔÚÈ«ÏØ303¸ö´å£¨ÉçÇø¡¢¾ÓÎ¯»á</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B101" t="inlineStr">
+        <is>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816133.html</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>央行报告:稳健的货币政策成效显著</t>
+        </is>
+      </c>
+      <c r="D101" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	　　本报北京8月9日电　（记者徐佩玉）中国人民银行6日发布的2020年第二季度中国货币政策执行报告指出，今年以来，稳健的货币政策成效显著，传导效率进一步提升，体现了前瞻性、精准性、主动性和有效性，金融支持实体经济力度明显增强。	　　今年以来，中国人民银行完善结构性货币政策工具体系，精准滴灌。目前，3000亿元专项再贷款和5000亿元再贷款、再贴现政策已基本执行完毕，1万亿元再贷款、再贴现政策有序衔接。同时，创新2项直达实体经济的政策工具，加大对普惠小微企业的支持力度。	　　报告透露，近期，中国人民银行对地方法人银行于今年3月1日至5月31日发放的符合</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816704.html</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>PPI环比上涨0.4%</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月10日电 （杨曦）国家统计局今日公布数据显示，2020年7月份，全国工业生产者出厂价格（PPI）同比下降2.4%，降幅比上月收窄0.6个百分点。从环比看，PPI上涨0.4%，涨幅与上月相同。	工业生产者购进价格同比下降3.3%，环比上涨0.9%。1至7月平均，工业生产者出厂价格比去年同期下降2.0%，工业生产者购进价格下降2.7%。工业生产者价格同比变动情况	工业生产者出厂价格中，生产资料价格同比下降3.5%，降幅比上月收窄0.7个百分点，影响工业生产者出厂价格总水平下降约2.56个百分点。其中，采掘工业价格下降7.1%，原材料工业价格</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816751.html</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>31省份最低工资:桂闽青已上调 京津沪暂缓</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	中国网财经8月10日讯(记者 畅帅帅)最低工资标准关系到每个人的钱袋子，尤其在疫情期间，更是为低收入人群的基本生活起到“兜底”作用。近期多省份提高失业保险金，而最低工资标准与失业保险金直接“挂钩”。	据中国网财经记者梳理，截至目前，共有青海、福建以及广西三地宣布上调最低工资标准，北京、上海、天津由于疫情原因，今年不作调整，其他省份暂未公布消息。	从排行榜来看，上海、北京、广东、天津、江苏、浙江等6省份月最低工资标准(指第一档标准，下同)超过2000元，上海以2480元的标准位列全国榜首。桂闽青今年已上调最低工资标准 京津沪暂缓调整	从最新调整动态来看</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	
+http://it.people.com.cn/n1/2020/0809/c1009-31815803.html</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>无人驾驶，距离载人上路还有多远？</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？赵超	自动避让行人、虚线变道超车、保持安全车距、处置复杂突发路况 …… 这些过去需要人小心完成的 “驾驶动作”，如今智能网联汽车也能“自动”实现。	今年4月20日，百度公司宣布旗下无人驾驶出租车服务 Apollo RoboTaxi 全面向长沙市民免费开放试乘。这些白色的纯电动智能网联汽车由百度阿波罗与中国一汽红旗联合研发，目前可在长沙梅溪湖国际文化艺术中心周边的街区行驶接客，吸引了不少尝鲜的市民前来体验、打卡。	近日，人民网记者赴长沙实地体验了一次无人驾驶出租车。据了解，无人驾驶技术近些年持续优化，并在商业化应用方面开始起步。但与此同时，围绕无人驾驶安</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>http://finance.people.com.cn/n1/2020/0810/c1004-31816159.html</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>超10万箱问题坚果流出 千亿市场亟待规范</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	日前，“10万余箱问题坚果流入市场”这一话题登上了微博热搜。	据央视财经报道，有消费者在网上花费126元购买了2盒国内某网红品牌的坚果，发现味道不对劲，于是选择报警。	警方在对网店展开调查后，于今年6月查处制假窝点。根据发货订单计算，犯罪嫌疑人以50元左右的价格，先后销售坚果共计10万余箱，300多万袋。	根据相应的打码视频素材，此次被假冒的网红品牌被大众指向了沃隆坚果。	8月5日和6日，沃隆坚果分别在其官方微博以及公众号上发布了致消费者的一封信，指出其打假办此前一直积极配合相应的调查工作，并提示消费者购买时要认准正规渠道。	8月6日下午，沃隆每日坚</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>http://world.people.com.cn/n1/2020/0810/c1002-31816277.html</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>新加坡夜空上演烟花秀 庆祝国庆日</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网讯 当地时间2020年8月9日，新加坡，新加坡上空燃起烟花，庆祝国庆日。	八月九日是新加坡的国庆日（National Day），这是纪念1965年新加坡独立的日子。 这一天全国人民会聚在一起，用声势浩大壮观的游行、集体舞蹈和大型烟花表演来庆祝这一日子。新加坡夜空上演烟花秀 庆祝国庆日优步在伦敦推出水上“打船”服务 有望替代地铁和公交车英国温莎城堡东露台花园40年来将首度向公众开放 “中东明珠”黎巴嫩 原来风景这么美！夏日避暑天堂 瑞典特色冰雪酒店看着都冷！ 巴勒斯坦民众玩转“焰火” 庆祝宰牲节  一起来赏月！“十五的月亮十四圆”现身多国夜空英国</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>http://world.people.com.cn/n1/2020/0809/c1002-31815629.html</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>贝鲁特粮仓被毁　联合国要向黎巴嫩运粮</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	　　世界粮食计划署7日说，将向黎巴嫩运送小麦和面粉等粮食，以应对黎巴嫩首都贝鲁特港口区大爆炸可能造成的粮食短缺。	　　大爆炸发生以前，国内金融危机和新冠疫情已经冲击黎巴嫩粮食供应。全国唯一一座位于港口的大型粮仓在爆炸中被毁，引发对黎巴嫩粮食安全的担忧。	　　【难以替代】	　　世界粮食计划署一名发言人在记者会上说，这一联合国机构担心大爆炸“将加剧（黎巴嫩）本已严峻的粮食安全状况”。	　　除运送粮食，世界粮食计划署还准备向黎巴嫩提供后勤等方面支持。	　　贝鲁特港口区4日傍晚发生剧烈爆炸，截至7日造成至少154人死亡、5000多人受伤，另有数十人失踪。据信</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>http://world.people.com.cn/n1/2020/0809/c1002-31815808.html</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>俄外交部发言人谴责美方打压抖音海外版</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	　　新华社莫斯科8月8日电 俄罗斯外交部发言人扎哈罗娃8日在莫斯科严词谴责美方打压抖音海外版（TikTok）的行为，认为这是美方不正当商业竞争的又一例证、违反了世界贸易组织规则。	　　据俄外交部网站消息，扎哈罗娃在评论抖音海外版在美遭遇时表示，美方基于空口无凭的指责，禁止美国公民与抖音海外版母公司字节跳动合作，并且咄咄逼人地强迫字节跳动把抖音海外版出售给美国企业。此举是美方为获取在国际信息领域的优势而采取不正当商业竞争的又一令人触目惊心的例证。“美国的这些行为与自由市场经济的基本原则背道而驰，违反了世界贸易组织规则。”	　　扎哈罗娃表示，俄方呼吁美方</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>http://world.people.com.cn/n1/2020/0809/c1002-31815809.html</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>特朗普绕开国会签署行政令延长失业救济</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	　　新华社华盛顿8月8日电（记者熊茂伶 高攀）在国会两党未谈拢新一轮财政援助的情况下，美国总统特朗普8日签署若干关于援助期限延期的行政令，其中包括延长已过期的额外失业救济金。	　　据美国媒体报道，特朗普绕过国会签署行政令的行为可能会遭遇法律挑战，因为美国宪法规定国会拥有支配联邦开支的权力。美国消费者新闻与商业频道报道认为，这可能既是特朗普的谈判策略，又是政治作秀，特朗普试图借此为其谋求连任造势。	　　按照国会3月底批准的新冠疫情纾困计划，联邦政府在各州失业救济金基础上，为失业人员提供的每周600美元额外失业救济金于7月底到期。特朗普新发布的行政令将把</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>http://world.people.com.cn/n1/2020/0810/c1002-31815957.html</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>英国同日本就“脱欧”后贸易谈判取得进展</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？本报驻英国记者  强  薇	　　日本外相茂木敏充8月5日至8日访问英国，与英方就“脱欧”后两国的贸易协定进行谈判，这是日本外相疫情后首次出访。英日双方表示，谈判取得“实质性进展”，但仍在一些关键领域存在分歧。	　　英国“脱欧”过渡期结束后，将不再享有此前欧盟和日本之间的贸易协定。这意味着，如果英日之间未能达成新的贸易协定，双方将于明年1月1日开始回到世界贸易组织框架下进行贸易。为此，双方于今年6月展开了贸易谈判。	　　根据英国政府的数据，去年英日两国之间的贸易总额为314亿英镑（1英镑约合1.3美元），英国有9500家企业向日本出口商品。日本是英国非欧</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>http://unn.people.com.cn/GB/393135/index.html</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>地方新闻</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？人民日报社概况|关于人民网|报社招聘|招聘英才|广告服务|合作加盟|供稿服务|网站声明|网站律师|信息保护|呼叫中心|ENGLISH镜像:日本  教育网  科技网  呼叫热线：4008-100-300  服务邮箱：kf@people.cn  违法和不良信息举报电话：010-65363263  举报邮箱：jubao@people.cn互联网新闻信息服务许可证10120170001|增值电信业务经营许可证B1-20060139信息网络传播视听节目许可证0104065|广播电视节目制作经营许可证（广媒）字第172号网络文化经营许可证            京</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>https://apiapp.people.cn/a/a/m/content_wap_263013.shtml</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>1分钟速看外交部回应美方错误言行</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>在现场 看世界 听未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>https://apiapp.people.cn/a/a/m/content_wap_263009.shtml</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>暖心大爷大妈为路边休息消防员擦背</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>在现场 看世界 听未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>https://apiapp.people.cn/a/a/m/content_wap_262943.shtml</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>燃!感受国之重器火箭炮的超强火力覆盖力</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>在现场 看世界 听未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>https://apiapp.people.cn/a/a/m/content_wap_262942.shtml</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>巴西海滩放气球纪念新冠肺炎逝者</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>在现场 看世界 听未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>https://apiapp.people.cn/a/a/m/content_wap_262990.shtml</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>女子骑摩托被撞倒 滚入路边下水道后消失</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>在现场 看世界 听未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>https://apiapp.people.cn/a/a/m/content_wap_262993.shtml</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>这款滚滚牌“椰香糯米糍”千万不能错过</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>在现场 看世界 听未来</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>http://leaders.people.com.cn/n1/2020/0810/c58278-31816642.html</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>湖北：多个景区人数达半年来“峰值”</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	8月8日、9日，是湖北启动“与爱同行 惠游湖北”活动后的首个周末，省文化和旅游厅统计，参加活动的全省364家A级旅游景区8月8日预约57.65万人，入园游览37.24万人。8月9日，十堰33家景区预约门票11.92万张，入园3.85万人。恩施州16家旅游景区共预约4.7万人，入园3.2万人，较8日预约增加2.1万人，入园增加1.3万人。	8月9日，武汉欢乐谷、武汉海昌极地海洋公园、黄鹤楼的门票9时许已预约完。黄鹤楼入园人数达2.5万人，比8日增长1倍。当日约8000名游客进入武当山景区，是半年来游客量的“峰值”。武当369国旅总经理徐勇干劲十足：“作</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>http://leaders.people.com.cn/n1/2020/0810/c58278-31816247.html</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>青海木里矿区非法开采 多人涉嫌失职失责</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	　　本报西宁8月9日电  （记者姜峰、王梅、贾丰丰）9日下午，青海省召开媒体报道木里矿区非法开采调查情况第二场新闻发布会。据介绍，经初步认定，涉事企业涉嫌违法违规，目前，海西蒙古族藏族自治州已有多人接受组织调查。	　　青海省委常委、省政府常务副省长李杰翔介绍，连日来，经现场踏查、科技勘查、账目资料审查及公安机关、纪委监委调查，初步认定，涉事企业涉嫌违法违规。目前，公安机关、纪委监委已成立专案组，对涉嫌违法违规行为和涉嫌失职失责等问题立案调查，调查进展情况将及时向社会和媒体公布。	　　青海省委常委、省纪委书记、省监委主任滕佳材介绍，经初步调查核实，时任</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>http://leaders.people.com.cn/n1/2020/0810/c58278-31816617.html</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>福建省首个乡镇农村产权服务中心成立</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	9日，（福建）全省首个乡镇农村产权服务中心在沙县夏茂镇挂牌成立。该中心的成立，将为社会资本进入农村产权交易市场提供基础数据和服务保障，标志着沙县农村产权交易服务进一步向乡、村两级延伸。	沙县有6万多人外出经营小吃，占农村劳动力的三分之二以上，农村普遍存在“人走房空、土地抛荒、林地失管”的现象。近年来，围绕小吃等特色产业发展和山区实际，沙县以入选全省首批县域集成改革试点为契机，探索实施“三票制”，即“房票”“地票”“林票”农村产权制度改革，盘活农村闲置房林地资源。	但由于农户和企业之间存在市场化水平差异大、信息不对称等问题，双方常出现对接无门、沟通不畅</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>http://leaders.people.com.cn/n1/2020/0810/c58278-31816579.html</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>辽宁14个县（市、区）启动试点“林长”制</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	为进一步加强山水林田湖草系统治理，促进全省生态环境保护与经济社会建设协调发展，并推进生态辽宁、美丽辽宁建设，我省在本溪、朝阳两市14县（市、区）启动林长制试点工作。林长制试点期为一年，之后全面推行。	据介绍，在试点市实行市、县、乡、村四级林长制，旨在强化党政领导，统筹山水林田湖草系统治理；突出森林（草原）资源的保护和发展，探索建立完整的林长制组织体系、明确的责任体系、健全的制度体系、科学的任务体系；有效解决林草行业当前面临的生态修复困难多、基础设施欠账多、产品供应能力弱等问题；积累好经验好做法，为全省推行林长制奠定坚实基础。	各级林长的主要职责，包括</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>http://unn.people.com.cn/difang/GB/387639/396439/index.html</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>专题|决战决胜脱贫攻坚地方策</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Ì«ÐÐÉ½ÂÌ£¬Î÷°ØÆÂºì£¡ÒÀ¿¿×ÅºìÓëÂÌÁ½ÖÖ×ÊÔ´£¬¸ïÃüÊ¥µØÎ÷°ØÆÂÕý·¢Éú×ÅÃÀÀöæÓ±ä£ºµ±µØ¼Ò¼Ò»§»§³ÔÉÏÁË¡°ÂÃÓÎ·¹¡±£¬ÎôÈÕµÄÍÁÅ÷·¿ÒÑ±äÉíÕû½àµÄÂ¥·¿¡¢±ðÊû£¬¶à°ëÅ©»§»¹¿ªÉÏÁËÐ¡½Î³µ¡£Î÷°ØÆÂµÄÏ²ÈË±ä»¯£¬ÊÇºÓ±±¾ÙÈ«Ê¡Ö®Á¦´òºÃÍÑÆ¶¹¥¼áÕ½µÄÒ»¸öËõÓ°¡£¡°´ÓÕÔ¼Ò¹µÏç¸ßÄÏ×¯´å°á½øÏØ³Ç¡®Íò¼ÒÀÖ¡¯°²ÖÃµã£¬ÎÒÏÂÂ¥ÓÃ²»ÁË10·ÖÖÓ¾ÍÄÜµ½³µ¼ä£¬</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>http://ah.people.com.cn/n2/2020/0810/c358266-34214939.html</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>直击怀宁汛后生产自救:工业农业“两手抓”</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	洪水退去，各地纷纷开启生产自救。	日前，记者在安徽省怀宁县看到，一边是农业大户抢抓时节、补栽补种；另一边，围绕工业企业复工复产的排除积涝、抢通水毁道路等工作，也正紧锣密鼓地进行中。全县上下，一派汛后生产自救忙的景象……	8月5日午后，怀宁县平山镇高泽村，蝉声盈耳，异常闷热。站在田边，即便什么活都不干，衣服上也会冒出盐渍。但村民王美凤顾不上这些，顶着烈日，她正忙着补栽秧苗。	王美凤，地道的农民。十多年前，她和丈夫开始流转耕地种水稻，这些年，又发展起稻虾共养。眼下，她流转的耕地接近2000亩，是不折不扣的农业大户。	前段日子，受持续强降雨影响，高泽村发生</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">
+http://hn.people.com.cn/n2/2020/0810/c337651-34216823.html</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>湖南两男子景区内漂流后下水游泳不幸溺亡</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网长沙8月10日电 据平江发布通报，8月8日，两名男子在湖南平江县连云山峡谷漂流景区漂流到达终点之后，脱去救生衣，擅自下水游泳，均不幸溺亡。	官方通报。网页截图关于连云山峡谷漂流发生一起意外溺亡事件的情况说明	2020年8月8日，钟某南（男，18岁，三阳乡白若村人）、湛某豪（男，18岁，汉昌镇北街人）等一行五人结伴去连云山峡谷漂流景区漂流。钟某南等人于12时起漂，到达终点后，钟某南、湛某豪两人脱去救生衣放在自助漂流皮筏上，擅自下水游泳，均意外溺亡。	事发后，平江县委、县政府高度重视，迅速成立由县文旅广体局、县应急管理局、县公安局、加义镇人民政府等</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>http://sc.people.com.cn/n2/2020/0810/c345509-34214989.html</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>9月1日起，成都对天然水域实施全面禁捕</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网成都8月10日电 据成都市农业农村局消息，近日，成都市农业农村局、成都市公安局、成都市市场监管局联合发布通告，明确从2020年9月1日0时起，对成都市天然水域实施全面禁捕，禁捕期暂定为10年。	禁捕期间，禁止任何组织和个人在天然水域范围内开展渔业资源的生产性捕捞。因特定渔业资源的利用和科研调查、苗种繁育等需要捕捞的，按照国家、省有关规定依法实行专项管理。	在禁捕范围和禁捕时间内，禁止违法从事天然渔业资源生产性捕捞，禁止使用拖网、围网、地笼网、罾网、滚钩等禁用渔具，禁止使用电、毒、炸等禁用方法捕捞，禁止收购、加工、销售、利用非法捕捞渔获物，禁止发</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>http://gx.people.com.cn/n2/2020/0810/c179430-34216652.html</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>广西培育产教融合型企业 加快产业转型升级</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿	Í¼ÎªÑ§ÉúÊµÑé³É¹ûÕ¹Ê¾¡£×ÔÖÎÇø·¢¸ÄÎ¯¹©Í¼	ÈËÃñÍøÄÏÄþ8ÔÂ10 ÈÕµç ½üÈÕ£¬ÎªÍÆ¶¯¹ãÎ÷²ú½ÌÈÚºÏÎÈ²½ÓÐÐò·¢Õ¹£¬¼Ó¿ìÅàÓý¡¢ÌáÉýÒ»ÅúÊ¾·¶´ø¶¯×÷ÓÃÇ¿µÄ²ú½ÌÈÚºÏÐÍÆóÒµ£¬¹ãÎ÷×³×å×ÔÖÎÇø·¢Õ¹ºÍ¸Ä¸ïÎ¯Ô±»áµÈ8²¿ÃÅÓ¡·¢ÁË¡¶¹ØÓÚ¹«²¼µÚÒ»Åú¹ãÎ÷²ú½ÌÈÚºÏÐÍÊÔµãÆóÒµÃûµ¥µÄÍ¨Öª¡·£¨ÏÂ³Æ¡¶Í¨Öª¡·£©£¬³É</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>http://ent.people.com.cn/n1/2020/0809/c1012-31815790.html</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>上海国际电影电视节贡献中国光影色彩</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？郭冠华 韦衍行	8月7日，为期14天的上海国际电影电视节落下帷幕。这是我国疫情防控常态化以来举办的首个电影电视节，在这个中国电影的发源地，人们尽享影视行业带来的美好，品味这场来之不易的光影盛宴。	2020年上海国际电影电视节的成功举办，不仅是“重逢”，更是“破圈”、“破局”。创新办节模式，影院展映、露天放映和线上放映三线并进，搭建国内外影视交流合作的云平台，本届上海电影电视节为影视行业的未来发展提出了独一无二的“上海方案”。开辟“云市场” 搭建影视交流平台	8月5日，上海国际电影节首次与电视节打通、共同推出的“国际影视云市场”圆满结束。在为期6天的时间</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>http://culture.people.com.cn/n1/2020/0810/c1013-31816331.html</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>各界助力故宫公共服务升级</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿Àîê»È¼¡¡¡¡Ëæ×ÅÔ½À´Ô½¶àµÄÓÎ¿ÍÄ½Ãû¶øÀ´£¬×öºÃ¹Å½¨Öþ±£»¤ÓëÌáÉý¹«¹²·þÎñÖÊÁ¿³ÉÎªÎÄ»¯ÒÅ²ú¾°ÇøÅ¬Á¦µÄÄ¿±ê¡£¡¡¡¡¡¡¡¡½üÈÕ£¬¡°¹Å½¨ÃÀ ÖÐ»ª»ê¡±¡ª¡ªÖÐ¹ú¹Å½¨ÖþÎÄ»¯½³ÐÄ´«³Ð¹«ÒæÐÐ¶¯¹Ê¹¬Õ¾ôß¹Ê¹¬²ÞËù¸ÄÔì¹«Òæ¾èÔùÏîÄ¿Ç©Ô¼ÒÇÊ½ÔÚ¹Ê¹¬²©ÎïÔº¾ÙÐÐ¡£¡¡¡¡Ç©Ô¼ÒÇÊ½ÉÏ£¬ÖÐ¹úÎÄÎï±£»¤»ù½ð»áÓë¹Ê¹¬²</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>http://culture.people.com.cn/n1/2020/0810/c1013-31816842.html</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>古代乐器在国博“奏响”丝竹之声</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿	ºÓÄÏÎèÑô¼ÖºþÐÂÊ¯Æ÷Ê±´úÎÄ»¯ÒÅÖ·³öÍÁµÄ¹ÇµÑ¡¢ÌÆ´ú¾ÅÏö»·ÅåÇÙ¡¢Çå´úÊ®¶þÂÉ¹Ü¡­¡­ÓÉÖÐ¹ú¹ú¼Ò²©Îï¹ÝÖ÷°ìµÄ¡°ÌìµØÍ¬ºÍ¡ª¡ªÖÐ¹ú¹Å´úÀÖÆ÷Õ¹¡±½üÈÕ¶Ô¹ÛÖÚ¿ª·Å£¬Á¦ÇóÏµÍ³·´Ó³ÖÐ¹ú¹Å´úÒôÀÖµÄ·¢Õ¹ÂöÂç£¬Õ¹ÏÖÖÐ¹ú´«Í³ÒôÀÖµÄÎÄ»¯¼ÛÖµ¡£	Õ¹ÀÀ·ÖÎª¡°º×Ãù¾Å¸Þ£¬ÉùÎÅÓÚÌì¡±¡°ÖÓ¹Ä†Å†Å£¬´óÒôÖÁÀÖ¡±¡°</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>http://culture.people.com.cn/n1/2020/0810/c1013-31815937.html</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>2020戏曲百戏（昆山）盛典10月开幕</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？　　本报南京8月9日电  （记者王伟健）记者获悉：2020戏曲百戏（昆山）盛典将于10月11日开幕，活动将举办19台大戏、20台折子戏、1场戏曲晚会。8月中旬起，主办方将开通线上线下售票渠道，活动将持续至11月下旬。　　据介绍，文化和旅游部艺术司、江苏省文化和旅游厅于2018年至2020年在昆山市共同举办3届百戏盛典。在前两年展演剧目的基础上，今年又有116个剧种、126个剧目来到昆山，从而实现3年集中展演全国348个戏曲剧种的经典剧目（折子戏）。自2018年戏曲百戏（昆山）盛典创新举办以来，先后组织了30个省（区、市）232个剧种、274个剧目、13</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>http://culture.people.com.cn/n1/2020/0810/c1013-31816134.html</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>郑州图书馆：以阅读温暖城市</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>µÇÂ¼ÈËÃñÍøÍ¨ÐÐÖ¤    Á¢¼´×¢²áÍü¼ÇÃÜÂë£¿»Æ×Óº­	¡¡¡¡½²×ùÉ³Áú¡¢Ö÷²¥Áì¶Á¡¢»¥¶¯ÌåÑé¡¢Ó°ÊÓÐÀÉÍ¡¢´´ÒâÊÖ¹¤¡¢»æ±¾·ÖÏí¡¢ÅàÑøÐ¡Ð¡Ö¾Ô¸Õß¡­¡­ÕâÊÇÖ£ÖÝÍ¼Êé¹Ý×Ô2014Äê¿ª´´µÄ¡°Í¼ÀÖ¡±Æ·ÅÆÔÄ¶Á»î¶¯£¬ÖÁ½ñÒÑ³É¹¦¾Ù°ì500Óà³¡´Î¡£³ÉÁ¢ÓÚ1953ÄêµÄÖ£ÖÝÍ¼Êé¹Ý£¬½üÄêÀ´ÔÚ´´ÐÂµÄÂ·ÉÏ¼ÓËÙ±¼ÅÜ£¬»ý¼«½¨Éè¸»ÓÐ´´ÔìÐÔ¡¢³äÂúÉú»ú¡¢ÒÔ¶ÁÕßÎªÖÐÐÄµÄ</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>http://sports.people.com.cn/n1/2020/0810/c14820-31816333.html</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>中职篮总决赛 期待更多精彩</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？本报记者  范佳元					　　8月8日，球员在篮下拼抢。当日，广东队以88∶85战胜北京队，从而以2∶1的总比分淘汰对手，晋级本赛季中职篮总决赛。					　　新华社记者 李紫恒摄	　　核心阅读	　　2019―2020赛季中职篮总决赛将于8月11日晚开赛，比赛采取三战两胜制。一边是第十五次晋级总决赛的上赛季冠军广东队，一边是第八次闯入总决赛的辽宁队，期待两队为球迷奉献更加精彩的比赛。	　　	　　8月8日，2019―2020赛季CBA（中国男篮职业联赛）季后赛半决赛全部结束，晋级总决赛的是同样有着丰富经验和强大阵容的辽宁队和广东队。	　　总决赛将于8月</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>http://sports.people.com.cn/n1/2020/0810/c22149-31816190.html</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>首钢队惜败卫冕冠军广东队返京</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？宋翔	8日，广东东莞银行队球员易建联（右）在比赛中防守北京首钢队球员林书豪的进攻 供图/新华社	北京首钢队8日晚输给卫冕冠军广东队后，于9日中午乘高铁从青岛返回北京。很多北京球迷在北京南站自发地热情迎接球队归来。有球迷打出了横幅“英雄归来，辛苦了”。据悉，后卫外援林书豪因为几天后要在青岛参加活动，这次并未与球队一起回京。	8日晚，首钢队在第三场比赛中以三分的劣势败北，就此结束了本赛季的征战。首钢队在这个赛季经历了很多困难，尤其是在复赛前，外籍主教练雅尼斯无法按时归队，中方助理教练解立彬临时拿起教鞭，他们最后取得了前四的赛季成绩，这也是球队重建后的最好战</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>http://sports.people.com.cn/n1/2020/0810/c22155-31816219.html</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>担忧疫情风险 瓦林卡退出美网</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？褚鹏	　　昨天（9日），瑞士著名网球选手、三届大满贯冠军斯坦・瓦林卡发布声明，将退出今年的辛辛那提大师赛和之后的美网大满贯。他坦言，在目前的条件下，他不想在美国打球。	　　瑞士名将之前的世界排名最高来到第三。2016年瓦林卡在美网男单决赛中，击败17届大满贯冠军德约科维奇夺得了他唯一的美网冠军。但考虑到疫情状况，瓦林卡表示目前不想赴美参赛。“我只是不想在这种情况下去美国旅行。”瓦林卡表示，“考虑到我现在的年龄和职业生涯，我不能什么比赛都打。我宁愿留在这里，为红土赛季做准备。”	　　身处欧洲，瓦林卡赛季的主要参赛目标，仍是美网后随即开始的红土赛季。“如果</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>http://sports.people.com.cn/n1/2020/0810/c22148-31816406.html</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>索尔斯克亚：渴望率领曼联赢得冠军奖杯</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	　　新华社伦敦8月9日电 英超曼联队主教练索尔斯克亚9日接受英国媒体采访时表示，希望能够带领球队赢得本赛季欧罗巴联赛冠军，实现自己作为主教练帮助曼联夺冠的梦想。	　　“我有远大的目标，我的其中一个梦想就是作为教练带领曼联赢得冠军奖杯，那将是我生命中最荣耀的时刻，”索尔斯克亚说。	　　现年47岁的挪威人索尔斯克亚作为球员效力曼联期间曾六夺联赛冠军，两次赢得足总杯冠军，一次赢得欧冠联赛冠军。	　　作为主教练，索尔斯克亚本赛季率领曼联获得联赛第三名，在联赛杯和足总杯赛中均止步半决赛。目前欧罗巴联赛中曼联已经杀入八强，四分之一决赛的对手是来自丹麦的哥本哈根队</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>http://sports.people.com.cn/n1/2020/0810/c407727-31816355.html</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>冬残奥会竞赛项目知识介绍片：单板滑雪</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	近日，北京冬奥组委推出冬残奥会竞赛项目知识介绍片，推广普及冬残奥会知识。	冬残奥会竞赛项目知识介绍片共由6部短片组成，每部短片介绍一个竞赛大项，包括：残奥高山滑雪、残奥单板滑雪、残奥越野滑雪、残奥冬季两项、残奥冰球、轮椅冰壶等，阐释了竞赛规则、场地情况、器材装备、赛事赏析点等内容。每部短片时长均为3分钟左右，采取了生动活泼、寓教于乐的方式，诠释了冬残奥会项目的独特魅力，展现了残疾人运动员自强不息、拼搏进取的精神风貌。</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>http://news.people.com.cn/GB/28053/index.html</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>热点新闻</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t xml:space="preserve">人民日报社概况|关于人民网|报社招聘|招聘英才|广告服务|合作加盟|供稿服务|网站声明|网站律师|呼叫中心|ENGLISH镜像:日本  教育网  科技网  服务邮箱  kf@people.cn  违法和不良信息举报电话：010-65363263互联网新闻信息服务许可证1012006001|增值电信业务经营许可证B2-20100025信息网络传播视听节目许可证0104065|广播电视节目制作经营许可证（广媒）字第172号网络文化经营许可证 京网文[2014]2108-308号|互联网出版许可证（京）字039号|京ICP证000006号|京公网安备11000002000008号人 民 网 版 权 </t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0808/c1008-31815407.html</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>国务院安委办开展爆炸性重点管控品检查</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？人民网北京8月8日电（薄晨棣）记者从应急管理部获悉，为深刻吸取黎巴嫩贝鲁特“8・4”重大爆炸事件教训，国务院安委办立即专题部署开展硝酸铵等爆炸性重点管控化学品生产储存企业及港口货场明查暗访工作。8月7日，派出6个工作组，赴河北、山西、福建、山东、河南、陕西、云南、贵州、重庆、四川、甘肃等11个省份和天津、青岛、上海、宁波港等4个重点港口，重点抽查辖区内硝酸铵生产、储存数量大的企业、化工园区和涉及硝酸铵流向的港口货场。	此次明查暗访聚焦重点，强化举一反三，将深入硝酸铵等爆炸性化学品的生产储存企业、港口码头货场等作业现场，重点检查有关部署贯彻落实情况、企业</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0808/c1008-31815443.html</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>国家防办调度部署重点地区强降雨防范应对</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？人民网北京8月8日电 （薄晨棣）据预报，8月8日至9日，内蒙古东北部、黑龙江西部、江苏中北部、安徽中北部、河南东南部、湖北中南部、湖南北部、贵州北部、四川南部、云南西部、西藏东南部等地部分地区有大到暴雨。国家防办、应急管理部8日召开会商调度会，与水利部、自然资源部、中国气象局会商研判雨水汛情发展态势，视频连线安徽、山东、山西、陕西、江西等地防指，进一步调度部署重点地区强降雨防范应对和人员转移避险工作。国家防总秘书长、应急管理部副部长兼水利部副部长周学文主持会议。	会议要求，各级防指要继续强化责任落实，充分发挥防指统筹协调作用，进一步强化以行政首长负责制</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>http://society.people.com.cn/n1/2020/0808/c1008-31815311.html</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>全国铁路营业里程突破14万公里</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？人民网北京8月8日电 （薄晨棣）记者从中国国家铁路集团有限公司（下称国铁集团）获悉，7月份，全国铁路固定资产投资完成671亿元，同比增长3.6%，其中基建大中型项目投资完成499亿元，同比增长11.3%。截至2020年7月底，全国铁路营业里程达到14.14万公里，其中高铁3.6万公里。	国铁集团建设部负责同志介绍，7月份以来，铁路部门认真贯彻落实中央“六稳”“六保”决策部署，统筹疫情防控和铁路建设，加大重点工程项目施工组织力度，严格工程质量安全管控，集中力量抓好在建和开工项目，取得重要进展。	一是部分新线顺利投产。上海至苏州至南通铁路、安顺至六盘水高速</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>http://travel.people.com.cn/n1/2020/0808/c41570-31815206.html</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>多项政策加速旅游回暖 旅客出行意愿提升</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月8日电 （记者刘佳）随着国内跨省游的恢复，山东、湖北等多个省市景区门票的减免，各家航空公司“随心飞”产品的推出……这一系列政策和优惠的加持，让在家“憋”了许久的人们都开始蠢蠢欲动，加速了旅游业的回暖。	近日，针对8月民航旅客出行意愿，民航旅客服务评测平台CAPSE共收集13874份有效样本，发布2020年8月旅客出行意愿指数分析报告。报告显示，8月旅客出行意愿指数环比提升12%，同比降幅收窄，有商务和旅游出行安排旅客占比均上升。8月有出行安排旅客占比提升 	报告指出，8月旅客出行意愿指数环比7月上升12%，与国内机场吞吐量趋势接近。8月</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>http://www.people.com.cn/</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>http://bj.people.com.cn/n2/2020/0808/c14540-34213226.html</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>北京:个人随意倾倒建筑垃圾最高罚200元</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>登录人民网通行证    立即注册忘记密码？	人民网北京8月8日电（池梦蕊）居民装修过程中产生的建筑垃圾应如何处置？费用由谁承担？近日，北京市公布《北京市建筑垃圾处置管理规定》（以下简称《规定》）对相关内容予以明确，并将于今年10月1日起施行。	建筑垃圾是指新建、改建、扩建和拆除各类建筑物、构筑物、管网等，强制拆除违法建设以及装饰装修房屋过程中产生的弃土(包括但不限于开槽渣土、级配砂石)、弃料以及其他固体废物。《规定》明确，任何单位和个人不得随意倾倒、抛撒或者堆放建筑垃圾，不得将建筑垃圾与其他生活垃圾、危险废物混合，不得未经许可从事建筑垃圾运输、消纳等活动。	在《规定》第五章“法律责任”中，对上</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>http://paper.people.com.cn/rmrbhwb/paperindex.htm</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>http://paper.people.com.cn/rmrbhwb/paperindex.htm</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>http://paper.people.com.cn/rmrbhwb/paperindex.htm</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>NO CONTENT</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>http://paper.people.com.cn/rmrb/index.html</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>http://paper.people.com.cn/rmrb/index.html</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>http://paper.people.com.cn/rmrb/index.html</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>NO CONTENT</t>
         </is>
       </c>
     </row>

</xml_diff>